<commit_message>
Starter definition of tables and some queries
</commit_message>
<xml_diff>
--- a/assets/doku/DB tables.xlsx
+++ b/assets/doku/DB tables.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="52">
   <si>
     <t>Table</t>
   </si>
@@ -28,9 +28,6 @@
   </si>
   <si>
     <t>passwds</t>
-  </si>
-  <si>
-    <t>?</t>
   </si>
   <si>
     <t>shopping_list</t>
@@ -126,9 +123,6 @@
     <t>varchar(120)</t>
   </si>
   <si>
-    <t>varchar(500)</t>
-  </si>
-  <si>
     <t>foreign_key(shopping_list.item_name)</t>
   </si>
   <si>
@@ -147,22 +141,37 @@
     <t>med.type</t>
   </si>
   <si>
-    <t>varchar(250)</t>
-  </si>
-  <si>
     <t>results</t>
   </si>
   <si>
     <t>date</t>
   </si>
   <si>
-    <t>varchar(300)</t>
-  </si>
-  <si>
     <t>foreign_key(med_tests.med_test_name)</t>
   </si>
   <si>
     <t>registration_date</t>
+  </si>
+  <si>
+    <t>varchar(100)</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>varchar(255)</t>
+  </si>
+  <si>
+    <t>text</t>
+  </si>
+  <si>
+    <t>passwd</t>
+  </si>
+  <si>
+    <t>varchar(60)</t>
+  </si>
+  <si>
+    <t>blob</t>
   </si>
 </sst>
 </file>
@@ -1230,6 +1239,42 @@
         </a:p>
       </dgm:t>
     </dgm:pt>
+    <dgm:pt modelId="{AE8947B9-4DD1-4CBA-876B-A4D5D8B01A87}">
+      <dgm:prSet phldrT="[Tekst]"/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="pl-PL"/>
+            <a:t>passwds</a:t>
+          </a:r>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{89D5F964-69B4-4004-B7D0-88E04A580D4C}" type="parTrans" cxnId="{07549231-1028-4839-90EE-ED2D4CFA9008}">
+      <dgm:prSet/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="pl-PL"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{74E6B8B5-04F1-47B0-B758-FDE2DD2D1E84}" type="sibTrans" cxnId="{07549231-1028-4839-90EE-ED2D4CFA9008}">
+      <dgm:prSet/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="pl-PL"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
     <dgm:pt modelId="{2928310D-2CA9-4834-90E6-7BDF49776789}" type="pres">
       <dgm:prSet presAssocID="{0D581458-B5EE-4A7F-90FD-3F9112FA4B78}" presName="hierChild1" presStyleCnt="0">
         <dgm:presLayoutVars>
@@ -1242,58 +1287,6 @@
         </dgm:presLayoutVars>
       </dgm:prSet>
       <dgm:spPr/>
-    </dgm:pt>
-    <dgm:pt modelId="{B2DCFB66-D7FB-48ED-BCA0-9F369E1668C2}" type="pres">
-      <dgm:prSet presAssocID="{90625BEE-1CE8-4E94-BD93-26C691FBA331}" presName="hierRoot1" presStyleCnt="0">
-        <dgm:presLayoutVars>
-          <dgm:hierBranch val="init"/>
-        </dgm:presLayoutVars>
-      </dgm:prSet>
-      <dgm:spPr/>
-    </dgm:pt>
-    <dgm:pt modelId="{EAC19A42-ACBD-4DEC-9558-1A920DBAF4EA}" type="pres">
-      <dgm:prSet presAssocID="{90625BEE-1CE8-4E94-BD93-26C691FBA331}" presName="rootComposite1" presStyleCnt="0"/>
-      <dgm:spPr/>
-    </dgm:pt>
-    <dgm:pt modelId="{0508117B-3BAB-41D1-94DF-0CF04275C7FA}" type="pres">
-      <dgm:prSet presAssocID="{90625BEE-1CE8-4E94-BD93-26C691FBA331}" presName="rootText1" presStyleLbl="node0" presStyleIdx="0" presStyleCnt="1">
-        <dgm:presLayoutVars>
-          <dgm:chPref val="3"/>
-        </dgm:presLayoutVars>
-      </dgm:prSet>
-      <dgm:spPr/>
-    </dgm:pt>
-    <dgm:pt modelId="{96CAB6C0-43D1-4509-B5E4-801A2235C3C0}" type="pres">
-      <dgm:prSet presAssocID="{90625BEE-1CE8-4E94-BD93-26C691FBA331}" presName="rootConnector1" presStyleLbl="node1" presStyleIdx="0" presStyleCnt="0"/>
-      <dgm:spPr/>
-    </dgm:pt>
-    <dgm:pt modelId="{E11E15A6-B9E1-4464-ACAB-B8B240A9A4D9}" type="pres">
-      <dgm:prSet presAssocID="{90625BEE-1CE8-4E94-BD93-26C691FBA331}" presName="hierChild2" presStyleCnt="0"/>
-      <dgm:spPr/>
-    </dgm:pt>
-    <dgm:pt modelId="{D696FE8C-BF81-4065-B3CB-3252DA3B830C}" type="pres">
-      <dgm:prSet presAssocID="{C1626232-3005-446D-A578-0D8DD393590B}" presName="Name37" presStyleLbl="parChTrans1D2" presStyleIdx="0" presStyleCnt="4"/>
-      <dgm:spPr/>
-    </dgm:pt>
-    <dgm:pt modelId="{3FF93C02-FB21-425A-8DCA-C0A9555346D2}" type="pres">
-      <dgm:prSet presAssocID="{F869AEC1-1E83-4EF1-A608-2ED7273BDA79}" presName="hierRoot2" presStyleCnt="0">
-        <dgm:presLayoutVars>
-          <dgm:hierBranch val="init"/>
-        </dgm:presLayoutVars>
-      </dgm:prSet>
-      <dgm:spPr/>
-    </dgm:pt>
-    <dgm:pt modelId="{9A93AD35-FE2B-4975-AF87-C0635F74306A}" type="pres">
-      <dgm:prSet presAssocID="{F869AEC1-1E83-4EF1-A608-2ED7273BDA79}" presName="rootComposite" presStyleCnt="0"/>
-      <dgm:spPr/>
-    </dgm:pt>
-    <dgm:pt modelId="{C57A6536-4127-4AA1-8522-04474917B5F5}" type="pres">
-      <dgm:prSet presAssocID="{F869AEC1-1E83-4EF1-A608-2ED7273BDA79}" presName="rootText" presStyleLbl="node2" presStyleIdx="0" presStyleCnt="4">
-        <dgm:presLayoutVars>
-          <dgm:chPref val="3"/>
-        </dgm:presLayoutVars>
-      </dgm:prSet>
-      <dgm:spPr/>
       <dgm:t>
         <a:bodyPr/>
         <a:lstStyle/>
@@ -1302,36 +1295,20 @@
         </a:p>
       </dgm:t>
     </dgm:pt>
-    <dgm:pt modelId="{E326ADC5-C67D-47B5-8B70-410250FC4F45}" type="pres">
-      <dgm:prSet presAssocID="{F869AEC1-1E83-4EF1-A608-2ED7273BDA79}" presName="rootConnector" presStyleLbl="node2" presStyleIdx="0" presStyleCnt="4"/>
-      <dgm:spPr/>
-    </dgm:pt>
-    <dgm:pt modelId="{22FF37A6-18B0-4E17-9930-7DD84E9700DF}" type="pres">
-      <dgm:prSet presAssocID="{F869AEC1-1E83-4EF1-A608-2ED7273BDA79}" presName="hierChild4" presStyleCnt="0"/>
-      <dgm:spPr/>
-    </dgm:pt>
-    <dgm:pt modelId="{AA5E1272-79FE-4603-BF34-34867740E12E}" type="pres">
-      <dgm:prSet presAssocID="{F869AEC1-1E83-4EF1-A608-2ED7273BDA79}" presName="hierChild5" presStyleCnt="0"/>
-      <dgm:spPr/>
-    </dgm:pt>
-    <dgm:pt modelId="{8B733281-3DE3-4C42-A883-193A9A249CD6}" type="pres">
-      <dgm:prSet presAssocID="{23DA1795-4ACE-4459-B5FA-3766EB5DF9C5}" presName="Name37" presStyleLbl="parChTrans1D2" presStyleIdx="1" presStyleCnt="4"/>
-      <dgm:spPr/>
-    </dgm:pt>
-    <dgm:pt modelId="{75AFD5F6-2F24-454A-84AD-345A8872FBE7}" type="pres">
-      <dgm:prSet presAssocID="{656B0FA4-A7DA-4D70-9B17-633C6CD7B506}" presName="hierRoot2" presStyleCnt="0">
+    <dgm:pt modelId="{B2DCFB66-D7FB-48ED-BCA0-9F369E1668C2}" type="pres">
+      <dgm:prSet presAssocID="{90625BEE-1CE8-4E94-BD93-26C691FBA331}" presName="hierRoot1" presStyleCnt="0">
         <dgm:presLayoutVars>
           <dgm:hierBranch val="init"/>
         </dgm:presLayoutVars>
       </dgm:prSet>
       <dgm:spPr/>
     </dgm:pt>
-    <dgm:pt modelId="{02700540-4257-49C1-AF0C-43800D0FA059}" type="pres">
-      <dgm:prSet presAssocID="{656B0FA4-A7DA-4D70-9B17-633C6CD7B506}" presName="rootComposite" presStyleCnt="0"/>
-      <dgm:spPr/>
-    </dgm:pt>
-    <dgm:pt modelId="{638ED046-8A50-4647-BF8C-DC993BB3E9B8}" type="pres">
-      <dgm:prSet presAssocID="{656B0FA4-A7DA-4D70-9B17-633C6CD7B506}" presName="rootText" presStyleLbl="node2" presStyleIdx="1" presStyleCnt="4">
+    <dgm:pt modelId="{EAC19A42-ACBD-4DEC-9558-1A920DBAF4EA}" type="pres">
+      <dgm:prSet presAssocID="{90625BEE-1CE8-4E94-BD93-26C691FBA331}" presName="rootComposite1" presStyleCnt="0"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{0508117B-3BAB-41D1-94DF-0CF04275C7FA}" type="pres">
+      <dgm:prSet presAssocID="{90625BEE-1CE8-4E94-BD93-26C691FBA331}" presName="rootText1" presStyleLbl="node0" presStyleIdx="0" presStyleCnt="1">
         <dgm:presLayoutVars>
           <dgm:chPref val="3"/>
         </dgm:presLayoutVars>
@@ -1345,36 +1322,8 @@
         </a:p>
       </dgm:t>
     </dgm:pt>
-    <dgm:pt modelId="{BE5A54D6-F6AF-424F-9423-F66B0C5B6243}" type="pres">
-      <dgm:prSet presAssocID="{656B0FA4-A7DA-4D70-9B17-633C6CD7B506}" presName="rootConnector" presStyleLbl="node2" presStyleIdx="1" presStyleCnt="4"/>
-      <dgm:spPr/>
-    </dgm:pt>
-    <dgm:pt modelId="{D9C58D4D-5691-43F6-9CC9-46F6E9A8CC40}" type="pres">
-      <dgm:prSet presAssocID="{656B0FA4-A7DA-4D70-9B17-633C6CD7B506}" presName="hierChild4" presStyleCnt="0"/>
-      <dgm:spPr/>
-    </dgm:pt>
-    <dgm:pt modelId="{CCD8050B-E3A1-4D78-A2EC-AF861030206E}" type="pres">
-      <dgm:prSet presAssocID="{4FB2B5CC-B5E8-4444-9946-1293B3748920}" presName="Name37" presStyleLbl="parChTrans1D3" presStyleIdx="0" presStyleCnt="2"/>
-      <dgm:spPr/>
-    </dgm:pt>
-    <dgm:pt modelId="{91320BF6-D109-4A45-B16D-C705B74FD78D}" type="pres">
-      <dgm:prSet presAssocID="{A6185CF1-A6C9-4057-B034-F738C98E78D8}" presName="hierRoot2" presStyleCnt="0">
-        <dgm:presLayoutVars>
-          <dgm:hierBranch val="init"/>
-        </dgm:presLayoutVars>
-      </dgm:prSet>
-      <dgm:spPr/>
-    </dgm:pt>
-    <dgm:pt modelId="{11538DA3-0FFC-4D24-8D5B-B452CCE01884}" type="pres">
-      <dgm:prSet presAssocID="{A6185CF1-A6C9-4057-B034-F738C98E78D8}" presName="rootComposite" presStyleCnt="0"/>
-      <dgm:spPr/>
-    </dgm:pt>
-    <dgm:pt modelId="{488D30EC-5368-42BE-91A5-E867C0D7A783}" type="pres">
-      <dgm:prSet presAssocID="{A6185CF1-A6C9-4057-B034-F738C98E78D8}" presName="rootText" presStyleLbl="node3" presStyleIdx="0" presStyleCnt="2">
-        <dgm:presLayoutVars>
-          <dgm:chPref val="3"/>
-        </dgm:presLayoutVars>
-      </dgm:prSet>
+    <dgm:pt modelId="{96CAB6C0-43D1-4509-B5E4-801A2235C3C0}" type="pres">
+      <dgm:prSet presAssocID="{90625BEE-1CE8-4E94-BD93-26C691FBA331}" presName="rootConnector1" presStyleLbl="node1" presStyleIdx="0" presStyleCnt="0"/>
       <dgm:spPr/>
       <dgm:t>
         <a:bodyPr/>
@@ -1384,76 +1333,12 @@
         </a:p>
       </dgm:t>
     </dgm:pt>
-    <dgm:pt modelId="{32A9C23E-AD8C-4291-91FD-D6B43BE6B459}" type="pres">
-      <dgm:prSet presAssocID="{A6185CF1-A6C9-4057-B034-F738C98E78D8}" presName="rootConnector" presStyleLbl="node3" presStyleIdx="0" presStyleCnt="2"/>
-      <dgm:spPr/>
-    </dgm:pt>
-    <dgm:pt modelId="{E16D2A24-4E46-4D94-9851-37881F0781E6}" type="pres">
-      <dgm:prSet presAssocID="{A6185CF1-A6C9-4057-B034-F738C98E78D8}" presName="hierChild4" presStyleCnt="0"/>
-      <dgm:spPr/>
-    </dgm:pt>
-    <dgm:pt modelId="{E7F26332-31D7-4D14-887D-38AC3F6B542D}" type="pres">
-      <dgm:prSet presAssocID="{A6185CF1-A6C9-4057-B034-F738C98E78D8}" presName="hierChild5" presStyleCnt="0"/>
-      <dgm:spPr/>
-    </dgm:pt>
-    <dgm:pt modelId="{5196F5DF-44C1-47A9-A6ED-F4D25A01B422}" type="pres">
-      <dgm:prSet presAssocID="{656B0FA4-A7DA-4D70-9B17-633C6CD7B506}" presName="hierChild5" presStyleCnt="0"/>
-      <dgm:spPr/>
-    </dgm:pt>
-    <dgm:pt modelId="{2E25BBEA-DA4E-4795-AB2E-4E623A9015ED}" type="pres">
-      <dgm:prSet presAssocID="{194D08C5-57EB-4155-B6F2-C4119AFD4E36}" presName="Name37" presStyleLbl="parChTrans1D2" presStyleIdx="2" presStyleCnt="4"/>
-      <dgm:spPr/>
-    </dgm:pt>
-    <dgm:pt modelId="{75E405C0-9842-4565-8FB6-DDB1CAFFD11A}" type="pres">
-      <dgm:prSet presAssocID="{50773849-F511-4835-AD5C-FC578FA128E4}" presName="hierRoot2" presStyleCnt="0">
-        <dgm:presLayoutVars>
-          <dgm:hierBranch val="init"/>
-        </dgm:presLayoutVars>
-      </dgm:prSet>
-      <dgm:spPr/>
-    </dgm:pt>
-    <dgm:pt modelId="{C7823C8D-F1A4-41A9-AAC6-90587AC45B04}" type="pres">
-      <dgm:prSet presAssocID="{50773849-F511-4835-AD5C-FC578FA128E4}" presName="rootComposite" presStyleCnt="0"/>
-      <dgm:spPr/>
-    </dgm:pt>
-    <dgm:pt modelId="{747F2FED-B883-4887-A704-3213D63B59EB}" type="pres">
-      <dgm:prSet presAssocID="{50773849-F511-4835-AD5C-FC578FA128E4}" presName="rootText" presStyleLbl="node2" presStyleIdx="2" presStyleCnt="4">
-        <dgm:presLayoutVars>
-          <dgm:chPref val="3"/>
-        </dgm:presLayoutVars>
-      </dgm:prSet>
-      <dgm:spPr/>
-    </dgm:pt>
-    <dgm:pt modelId="{D09303C9-BCC6-4DD2-8E33-C0F1AE38C831}" type="pres">
-      <dgm:prSet presAssocID="{50773849-F511-4835-AD5C-FC578FA128E4}" presName="rootConnector" presStyleLbl="node2" presStyleIdx="2" presStyleCnt="4"/>
-      <dgm:spPr/>
-    </dgm:pt>
-    <dgm:pt modelId="{8FCEA839-5421-4B25-A77C-B2B6C2C02558}" type="pres">
-      <dgm:prSet presAssocID="{50773849-F511-4835-AD5C-FC578FA128E4}" presName="hierChild4" presStyleCnt="0"/>
-      <dgm:spPr/>
-    </dgm:pt>
-    <dgm:pt modelId="{F4C3505A-509D-492B-A76D-03D866D48A9B}" type="pres">
-      <dgm:prSet presAssocID="{237A5FB3-0392-40DF-98C3-051D76C85975}" presName="Name37" presStyleLbl="parChTrans1D3" presStyleIdx="1" presStyleCnt="2"/>
-      <dgm:spPr/>
-    </dgm:pt>
-    <dgm:pt modelId="{6C87BF26-6704-4F24-B5DC-5F0E523ACA4C}" type="pres">
-      <dgm:prSet presAssocID="{B56F1F7B-9CAF-4E3C-8845-E5A0D88E4AC1}" presName="hierRoot2" presStyleCnt="0">
-        <dgm:presLayoutVars>
-          <dgm:hierBranch val="init"/>
-        </dgm:presLayoutVars>
-      </dgm:prSet>
-      <dgm:spPr/>
-    </dgm:pt>
-    <dgm:pt modelId="{AC6E90D5-E063-42D9-84FA-641E716E09D9}" type="pres">
-      <dgm:prSet presAssocID="{B56F1F7B-9CAF-4E3C-8845-E5A0D88E4AC1}" presName="rootComposite" presStyleCnt="0"/>
-      <dgm:spPr/>
-    </dgm:pt>
-    <dgm:pt modelId="{C9C249D0-F1D4-4554-A386-CAFA14270C36}" type="pres">
-      <dgm:prSet presAssocID="{B56F1F7B-9CAF-4E3C-8845-E5A0D88E4AC1}" presName="rootText" presStyleLbl="node3" presStyleIdx="1" presStyleCnt="2">
-        <dgm:presLayoutVars>
-          <dgm:chPref val="3"/>
-        </dgm:presLayoutVars>
-      </dgm:prSet>
+    <dgm:pt modelId="{E11E15A6-B9E1-4464-ACAB-B8B240A9A4D9}" type="pres">
+      <dgm:prSet presAssocID="{90625BEE-1CE8-4E94-BD93-26C691FBA331}" presName="hierChild2" presStyleCnt="0"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{D696FE8C-BF81-4065-B3CB-3252DA3B830C}" type="pres">
+      <dgm:prSet presAssocID="{C1626232-3005-446D-A578-0D8DD393590B}" presName="Name37" presStyleLbl="parChTrans1D2" presStyleIdx="0" presStyleCnt="5"/>
       <dgm:spPr/>
       <dgm:t>
         <a:bodyPr/>
@@ -1463,40 +1348,20 @@
         </a:p>
       </dgm:t>
     </dgm:pt>
-    <dgm:pt modelId="{FFF9F715-5053-4613-89FA-1E0570F1C0C0}" type="pres">
-      <dgm:prSet presAssocID="{B56F1F7B-9CAF-4E3C-8845-E5A0D88E4AC1}" presName="rootConnector" presStyleLbl="node3" presStyleIdx="1" presStyleCnt="2"/>
-      <dgm:spPr/>
-    </dgm:pt>
-    <dgm:pt modelId="{803497FD-6163-4B62-AAA2-735D49D988DD}" type="pres">
-      <dgm:prSet presAssocID="{B56F1F7B-9CAF-4E3C-8845-E5A0D88E4AC1}" presName="hierChild4" presStyleCnt="0"/>
-      <dgm:spPr/>
-    </dgm:pt>
-    <dgm:pt modelId="{ACDCB1B2-5443-4038-80D4-CE277A515A25}" type="pres">
-      <dgm:prSet presAssocID="{B56F1F7B-9CAF-4E3C-8845-E5A0D88E4AC1}" presName="hierChild5" presStyleCnt="0"/>
-      <dgm:spPr/>
-    </dgm:pt>
-    <dgm:pt modelId="{B0CFFD3F-A927-4D27-97EA-5C803C05C1EC}" type="pres">
-      <dgm:prSet presAssocID="{50773849-F511-4835-AD5C-FC578FA128E4}" presName="hierChild5" presStyleCnt="0"/>
-      <dgm:spPr/>
-    </dgm:pt>
-    <dgm:pt modelId="{F2B1825C-8BC8-4111-A2C0-A0FBB338DE48}" type="pres">
-      <dgm:prSet presAssocID="{03BF1FA9-C075-4FA8-BD05-B802322534A6}" presName="Name37" presStyleLbl="parChTrans1D2" presStyleIdx="3" presStyleCnt="4"/>
-      <dgm:spPr/>
-    </dgm:pt>
-    <dgm:pt modelId="{2F6718CB-1A8A-4650-AB72-E9A1BE671FFE}" type="pres">
-      <dgm:prSet presAssocID="{862D7E0D-F0D4-41D7-97A9-5B92A6FAF196}" presName="hierRoot2" presStyleCnt="0">
+    <dgm:pt modelId="{3FF93C02-FB21-425A-8DCA-C0A9555346D2}" type="pres">
+      <dgm:prSet presAssocID="{F869AEC1-1E83-4EF1-A608-2ED7273BDA79}" presName="hierRoot2" presStyleCnt="0">
         <dgm:presLayoutVars>
           <dgm:hierBranch val="init"/>
         </dgm:presLayoutVars>
       </dgm:prSet>
       <dgm:spPr/>
     </dgm:pt>
-    <dgm:pt modelId="{1C50B8F7-B0D8-4AC7-9697-96D6DC8A6695}" type="pres">
-      <dgm:prSet presAssocID="{862D7E0D-F0D4-41D7-97A9-5B92A6FAF196}" presName="rootComposite" presStyleCnt="0"/>
-      <dgm:spPr/>
-    </dgm:pt>
-    <dgm:pt modelId="{B4A89E68-830E-49C7-8936-A684A6D977A9}" type="pres">
-      <dgm:prSet presAssocID="{862D7E0D-F0D4-41D7-97A9-5B92A6FAF196}" presName="rootText" presStyleLbl="node2" presStyleIdx="3" presStyleCnt="4">
+    <dgm:pt modelId="{9A93AD35-FE2B-4975-AF87-C0635F74306A}" type="pres">
+      <dgm:prSet presAssocID="{F869AEC1-1E83-4EF1-A608-2ED7273BDA79}" presName="rootComposite" presStyleCnt="0"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{C57A6536-4127-4AA1-8522-04474917B5F5}" type="pres">
+      <dgm:prSet presAssocID="{F869AEC1-1E83-4EF1-A608-2ED7273BDA79}" presName="rootText" presStyleLbl="node2" presStyleIdx="0" presStyleCnt="5">
         <dgm:presLayoutVars>
           <dgm:chPref val="3"/>
         </dgm:presLayoutVars>
@@ -1510,9 +1375,301 @@
         </a:p>
       </dgm:t>
     </dgm:pt>
+    <dgm:pt modelId="{E326ADC5-C67D-47B5-8B70-410250FC4F45}" type="pres">
+      <dgm:prSet presAssocID="{F869AEC1-1E83-4EF1-A608-2ED7273BDA79}" presName="rootConnector" presStyleLbl="node2" presStyleIdx="0" presStyleCnt="5"/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="pl-PL"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{22FF37A6-18B0-4E17-9930-7DD84E9700DF}" type="pres">
+      <dgm:prSet presAssocID="{F869AEC1-1E83-4EF1-A608-2ED7273BDA79}" presName="hierChild4" presStyleCnt="0"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{AA5E1272-79FE-4603-BF34-34867740E12E}" type="pres">
+      <dgm:prSet presAssocID="{F869AEC1-1E83-4EF1-A608-2ED7273BDA79}" presName="hierChild5" presStyleCnt="0"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{8B733281-3DE3-4C42-A883-193A9A249CD6}" type="pres">
+      <dgm:prSet presAssocID="{23DA1795-4ACE-4459-B5FA-3766EB5DF9C5}" presName="Name37" presStyleLbl="parChTrans1D2" presStyleIdx="1" presStyleCnt="5"/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="pl-PL"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{75AFD5F6-2F24-454A-84AD-345A8872FBE7}" type="pres">
+      <dgm:prSet presAssocID="{656B0FA4-A7DA-4D70-9B17-633C6CD7B506}" presName="hierRoot2" presStyleCnt="0">
+        <dgm:presLayoutVars>
+          <dgm:hierBranch val="init"/>
+        </dgm:presLayoutVars>
+      </dgm:prSet>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{02700540-4257-49C1-AF0C-43800D0FA059}" type="pres">
+      <dgm:prSet presAssocID="{656B0FA4-A7DA-4D70-9B17-633C6CD7B506}" presName="rootComposite" presStyleCnt="0"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{638ED046-8A50-4647-BF8C-DC993BB3E9B8}" type="pres">
+      <dgm:prSet presAssocID="{656B0FA4-A7DA-4D70-9B17-633C6CD7B506}" presName="rootText" presStyleLbl="node2" presStyleIdx="1" presStyleCnt="5">
+        <dgm:presLayoutVars>
+          <dgm:chPref val="3"/>
+        </dgm:presLayoutVars>
+      </dgm:prSet>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="pl-PL"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{BE5A54D6-F6AF-424F-9423-F66B0C5B6243}" type="pres">
+      <dgm:prSet presAssocID="{656B0FA4-A7DA-4D70-9B17-633C6CD7B506}" presName="rootConnector" presStyleLbl="node2" presStyleIdx="1" presStyleCnt="5"/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="pl-PL"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{D9C58D4D-5691-43F6-9CC9-46F6E9A8CC40}" type="pres">
+      <dgm:prSet presAssocID="{656B0FA4-A7DA-4D70-9B17-633C6CD7B506}" presName="hierChild4" presStyleCnt="0"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{CCD8050B-E3A1-4D78-A2EC-AF861030206E}" type="pres">
+      <dgm:prSet presAssocID="{4FB2B5CC-B5E8-4444-9946-1293B3748920}" presName="Name37" presStyleLbl="parChTrans1D3" presStyleIdx="0" presStyleCnt="2"/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="pl-PL"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{91320BF6-D109-4A45-B16D-C705B74FD78D}" type="pres">
+      <dgm:prSet presAssocID="{A6185CF1-A6C9-4057-B034-F738C98E78D8}" presName="hierRoot2" presStyleCnt="0">
+        <dgm:presLayoutVars>
+          <dgm:hierBranch val="init"/>
+        </dgm:presLayoutVars>
+      </dgm:prSet>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{11538DA3-0FFC-4D24-8D5B-B452CCE01884}" type="pres">
+      <dgm:prSet presAssocID="{A6185CF1-A6C9-4057-B034-F738C98E78D8}" presName="rootComposite" presStyleCnt="0"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{488D30EC-5368-42BE-91A5-E867C0D7A783}" type="pres">
+      <dgm:prSet presAssocID="{A6185CF1-A6C9-4057-B034-F738C98E78D8}" presName="rootText" presStyleLbl="node3" presStyleIdx="0" presStyleCnt="2">
+        <dgm:presLayoutVars>
+          <dgm:chPref val="3"/>
+        </dgm:presLayoutVars>
+      </dgm:prSet>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="pl-PL"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{32A9C23E-AD8C-4291-91FD-D6B43BE6B459}" type="pres">
+      <dgm:prSet presAssocID="{A6185CF1-A6C9-4057-B034-F738C98E78D8}" presName="rootConnector" presStyleLbl="node3" presStyleIdx="0" presStyleCnt="2"/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="pl-PL"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{E16D2A24-4E46-4D94-9851-37881F0781E6}" type="pres">
+      <dgm:prSet presAssocID="{A6185CF1-A6C9-4057-B034-F738C98E78D8}" presName="hierChild4" presStyleCnt="0"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{E7F26332-31D7-4D14-887D-38AC3F6B542D}" type="pres">
+      <dgm:prSet presAssocID="{A6185CF1-A6C9-4057-B034-F738C98E78D8}" presName="hierChild5" presStyleCnt="0"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{5196F5DF-44C1-47A9-A6ED-F4D25A01B422}" type="pres">
+      <dgm:prSet presAssocID="{656B0FA4-A7DA-4D70-9B17-633C6CD7B506}" presName="hierChild5" presStyleCnt="0"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{2E25BBEA-DA4E-4795-AB2E-4E623A9015ED}" type="pres">
+      <dgm:prSet presAssocID="{194D08C5-57EB-4155-B6F2-C4119AFD4E36}" presName="Name37" presStyleLbl="parChTrans1D2" presStyleIdx="2" presStyleCnt="5"/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="pl-PL"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{75E405C0-9842-4565-8FB6-DDB1CAFFD11A}" type="pres">
+      <dgm:prSet presAssocID="{50773849-F511-4835-AD5C-FC578FA128E4}" presName="hierRoot2" presStyleCnt="0">
+        <dgm:presLayoutVars>
+          <dgm:hierBranch val="init"/>
+        </dgm:presLayoutVars>
+      </dgm:prSet>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{C7823C8D-F1A4-41A9-AAC6-90587AC45B04}" type="pres">
+      <dgm:prSet presAssocID="{50773849-F511-4835-AD5C-FC578FA128E4}" presName="rootComposite" presStyleCnt="0"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{747F2FED-B883-4887-A704-3213D63B59EB}" type="pres">
+      <dgm:prSet presAssocID="{50773849-F511-4835-AD5C-FC578FA128E4}" presName="rootText" presStyleLbl="node2" presStyleIdx="2" presStyleCnt="5">
+        <dgm:presLayoutVars>
+          <dgm:chPref val="3"/>
+        </dgm:presLayoutVars>
+      </dgm:prSet>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="pl-PL"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{D09303C9-BCC6-4DD2-8E33-C0F1AE38C831}" type="pres">
+      <dgm:prSet presAssocID="{50773849-F511-4835-AD5C-FC578FA128E4}" presName="rootConnector" presStyleLbl="node2" presStyleIdx="2" presStyleCnt="5"/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="pl-PL"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{8FCEA839-5421-4B25-A77C-B2B6C2C02558}" type="pres">
+      <dgm:prSet presAssocID="{50773849-F511-4835-AD5C-FC578FA128E4}" presName="hierChild4" presStyleCnt="0"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{F4C3505A-509D-492B-A76D-03D866D48A9B}" type="pres">
+      <dgm:prSet presAssocID="{237A5FB3-0392-40DF-98C3-051D76C85975}" presName="Name37" presStyleLbl="parChTrans1D3" presStyleIdx="1" presStyleCnt="2"/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="pl-PL"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{6C87BF26-6704-4F24-B5DC-5F0E523ACA4C}" type="pres">
+      <dgm:prSet presAssocID="{B56F1F7B-9CAF-4E3C-8845-E5A0D88E4AC1}" presName="hierRoot2" presStyleCnt="0">
+        <dgm:presLayoutVars>
+          <dgm:hierBranch val="init"/>
+        </dgm:presLayoutVars>
+      </dgm:prSet>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{AC6E90D5-E063-42D9-84FA-641E716E09D9}" type="pres">
+      <dgm:prSet presAssocID="{B56F1F7B-9CAF-4E3C-8845-E5A0D88E4AC1}" presName="rootComposite" presStyleCnt="0"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{C9C249D0-F1D4-4554-A386-CAFA14270C36}" type="pres">
+      <dgm:prSet presAssocID="{B56F1F7B-9CAF-4E3C-8845-E5A0D88E4AC1}" presName="rootText" presStyleLbl="node3" presStyleIdx="1" presStyleCnt="2">
+        <dgm:presLayoutVars>
+          <dgm:chPref val="3"/>
+        </dgm:presLayoutVars>
+      </dgm:prSet>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="pl-PL"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{FFF9F715-5053-4613-89FA-1E0570F1C0C0}" type="pres">
+      <dgm:prSet presAssocID="{B56F1F7B-9CAF-4E3C-8845-E5A0D88E4AC1}" presName="rootConnector" presStyleLbl="node3" presStyleIdx="1" presStyleCnt="2"/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="pl-PL"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{803497FD-6163-4B62-AAA2-735D49D988DD}" type="pres">
+      <dgm:prSet presAssocID="{B56F1F7B-9CAF-4E3C-8845-E5A0D88E4AC1}" presName="hierChild4" presStyleCnt="0"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{ACDCB1B2-5443-4038-80D4-CE277A515A25}" type="pres">
+      <dgm:prSet presAssocID="{B56F1F7B-9CAF-4E3C-8845-E5A0D88E4AC1}" presName="hierChild5" presStyleCnt="0"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{B0CFFD3F-A927-4D27-97EA-5C803C05C1EC}" type="pres">
+      <dgm:prSet presAssocID="{50773849-F511-4835-AD5C-FC578FA128E4}" presName="hierChild5" presStyleCnt="0"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{F2B1825C-8BC8-4111-A2C0-A0FBB338DE48}" type="pres">
+      <dgm:prSet presAssocID="{03BF1FA9-C075-4FA8-BD05-B802322534A6}" presName="Name37" presStyleLbl="parChTrans1D2" presStyleIdx="3" presStyleCnt="5"/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="pl-PL"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{2F6718CB-1A8A-4650-AB72-E9A1BE671FFE}" type="pres">
+      <dgm:prSet presAssocID="{862D7E0D-F0D4-41D7-97A9-5B92A6FAF196}" presName="hierRoot2" presStyleCnt="0">
+        <dgm:presLayoutVars>
+          <dgm:hierBranch val="init"/>
+        </dgm:presLayoutVars>
+      </dgm:prSet>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{1C50B8F7-B0D8-4AC7-9697-96D6DC8A6695}" type="pres">
+      <dgm:prSet presAssocID="{862D7E0D-F0D4-41D7-97A9-5B92A6FAF196}" presName="rootComposite" presStyleCnt="0"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{B4A89E68-830E-49C7-8936-A684A6D977A9}" type="pres">
+      <dgm:prSet presAssocID="{862D7E0D-F0D4-41D7-97A9-5B92A6FAF196}" presName="rootText" presStyleLbl="node2" presStyleIdx="3" presStyleCnt="5">
+        <dgm:presLayoutVars>
+          <dgm:chPref val="3"/>
+        </dgm:presLayoutVars>
+      </dgm:prSet>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="pl-PL"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
     <dgm:pt modelId="{00785835-E3F4-4EF8-924A-607B1BE17BA3}" type="pres">
-      <dgm:prSet presAssocID="{862D7E0D-F0D4-41D7-97A9-5B92A6FAF196}" presName="rootConnector" presStyleLbl="node2" presStyleIdx="3" presStyleCnt="4"/>
-      <dgm:spPr/>
+      <dgm:prSet presAssocID="{862D7E0D-F0D4-41D7-97A9-5B92A6FAF196}" presName="rootConnector" presStyleLbl="node2" presStyleIdx="3" presStyleCnt="5"/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="pl-PL"/>
+        </a:p>
+      </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{7CDF85EA-A31C-46FE-AC6A-AA3C59759A2A}" type="pres">
       <dgm:prSet presAssocID="{862D7E0D-F0D4-41D7-97A9-5B92A6FAF196}" presName="hierChild4" presStyleCnt="0"/>
@@ -1522,40 +1679,94 @@
       <dgm:prSet presAssocID="{862D7E0D-F0D4-41D7-97A9-5B92A6FAF196}" presName="hierChild5" presStyleCnt="0"/>
       <dgm:spPr/>
     </dgm:pt>
+    <dgm:pt modelId="{993DFE86-1DCA-48E6-AB6D-7101F7F884D6}" type="pres">
+      <dgm:prSet presAssocID="{89D5F964-69B4-4004-B7D0-88E04A580D4C}" presName="Name37" presStyleLbl="parChTrans1D2" presStyleIdx="4" presStyleCnt="5"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{C8B37CB4-59A5-4030-AA67-752675154247}" type="pres">
+      <dgm:prSet presAssocID="{AE8947B9-4DD1-4CBA-876B-A4D5D8B01A87}" presName="hierRoot2" presStyleCnt="0">
+        <dgm:presLayoutVars>
+          <dgm:hierBranch val="init"/>
+        </dgm:presLayoutVars>
+      </dgm:prSet>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{17CD3FE5-42A0-4E0F-9D5C-426B3CBDC113}" type="pres">
+      <dgm:prSet presAssocID="{AE8947B9-4DD1-4CBA-876B-A4D5D8B01A87}" presName="rootComposite" presStyleCnt="0"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{77618643-8909-4B96-B865-0D76F6C6AC5C}" type="pres">
+      <dgm:prSet presAssocID="{AE8947B9-4DD1-4CBA-876B-A4D5D8B01A87}" presName="rootText" presStyleLbl="node2" presStyleIdx="4" presStyleCnt="5">
+        <dgm:presLayoutVars>
+          <dgm:chPref val="3"/>
+        </dgm:presLayoutVars>
+      </dgm:prSet>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="pl-PL"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{82DF419B-8EE6-4CB7-BAB1-86FC9D1E9AC1}" type="pres">
+      <dgm:prSet presAssocID="{AE8947B9-4DD1-4CBA-876B-A4D5D8B01A87}" presName="rootConnector" presStyleLbl="node2" presStyleIdx="4" presStyleCnt="5"/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="pl-PL"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{AB06BFB8-3302-441D-AE77-152478D7B0A2}" type="pres">
+      <dgm:prSet presAssocID="{AE8947B9-4DD1-4CBA-876B-A4D5D8B01A87}" presName="hierChild4" presStyleCnt="0"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{7652BEC3-3C8D-48EA-9EA3-3C49EBEB8780}" type="pres">
+      <dgm:prSet presAssocID="{AE8947B9-4DD1-4CBA-876B-A4D5D8B01A87}" presName="hierChild5" presStyleCnt="0"/>
+      <dgm:spPr/>
+    </dgm:pt>
     <dgm:pt modelId="{62033BBF-FDB7-402B-8DA8-A036D51728D0}" type="pres">
       <dgm:prSet presAssocID="{90625BEE-1CE8-4E94-BD93-26C691FBA331}" presName="hierChild3" presStyleCnt="0"/>
       <dgm:spPr/>
     </dgm:pt>
   </dgm:ptLst>
   <dgm:cxnLst>
+    <dgm:cxn modelId="{8BE19EC5-B58E-4BB9-94F6-ED249D783BE0}" type="presOf" srcId="{F869AEC1-1E83-4EF1-A608-2ED7273BDA79}" destId="{E326ADC5-C67D-47B5-8B70-410250FC4F45}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{0571FFFF-892A-4489-BC21-50013D5FAFB8}" type="presOf" srcId="{656B0FA4-A7DA-4D70-9B17-633C6CD7B506}" destId="{BE5A54D6-F6AF-424F-9423-F66B0C5B6243}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{DD52EC3C-F2CD-484A-9560-578DFDD6F601}" type="presOf" srcId="{B56F1F7B-9CAF-4E3C-8845-E5A0D88E4AC1}" destId="{C9C249D0-F1D4-4554-A386-CAFA14270C36}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{71E0349D-088D-4E65-A8C6-D6879D89E856}" type="presOf" srcId="{03BF1FA9-C075-4FA8-BD05-B802322534A6}" destId="{F2B1825C-8BC8-4111-A2C0-A0FBB338DE48}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{325DAB41-614B-4868-B08A-5032FB3CA0F3}" srcId="{50773849-F511-4835-AD5C-FC578FA128E4}" destId="{B56F1F7B-9CAF-4E3C-8845-E5A0D88E4AC1}" srcOrd="0" destOrd="0" parTransId="{237A5FB3-0392-40DF-98C3-051D76C85975}" sibTransId="{D9AC3E19-03F8-4B24-9C05-1F58DDABFDD4}"/>
+    <dgm:cxn modelId="{A02A8C92-53D2-400A-8E31-C1D36C74C310}" type="presOf" srcId="{A6185CF1-A6C9-4057-B034-F738C98E78D8}" destId="{488D30EC-5368-42BE-91A5-E867C0D7A783}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{B64F773A-90DB-49B8-A18F-5E4035FFF432}" srcId="{0D581458-B5EE-4A7F-90FD-3F9112FA4B78}" destId="{90625BEE-1CE8-4E94-BD93-26C691FBA331}" srcOrd="0" destOrd="0" parTransId="{0F3A10AD-3B79-4301-B641-B9A7875FF524}" sibTransId="{9544EE45-59CE-4B8F-A53E-FCC70B170D25}"/>
+    <dgm:cxn modelId="{02C98010-6CFF-47EB-983D-ABB138E78C3F}" type="presOf" srcId="{C1626232-3005-446D-A578-0D8DD393590B}" destId="{D696FE8C-BF81-4065-B3CB-3252DA3B830C}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{63E4C16F-DAFF-4115-824D-4E5062F2889B}" type="presOf" srcId="{90625BEE-1CE8-4E94-BD93-26C691FBA331}" destId="{0508117B-3BAB-41D1-94DF-0CF04275C7FA}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{58D39FB8-3B72-436D-B378-75D5CFD0C8F7}" srcId="{90625BEE-1CE8-4E94-BD93-26C691FBA331}" destId="{862D7E0D-F0D4-41D7-97A9-5B92A6FAF196}" srcOrd="3" destOrd="0" parTransId="{03BF1FA9-C075-4FA8-BD05-B802322534A6}" sibTransId="{C266CAE2-4D1C-4F15-A627-AE1D114514FC}"/>
+    <dgm:cxn modelId="{B0173BF3-1663-4869-9510-FF3E6ECDB80B}" type="presOf" srcId="{90625BEE-1CE8-4E94-BD93-26C691FBA331}" destId="{96CAB6C0-43D1-4509-B5E4-801A2235C3C0}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{C56E1D74-B152-4B9F-8564-CBCE6D400DF6}" type="presOf" srcId="{A6185CF1-A6C9-4057-B034-F738C98E78D8}" destId="{32A9C23E-AD8C-4291-91FD-D6B43BE6B459}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{1DD651EF-393A-4ECA-BDA5-58D00B75F246}" type="presOf" srcId="{194D08C5-57EB-4155-B6F2-C4119AFD4E36}" destId="{2E25BBEA-DA4E-4795-AB2E-4E623A9015ED}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{BF396FEA-265D-4E32-A5F2-137B0774A15F}" type="presOf" srcId="{AE8947B9-4DD1-4CBA-876B-A4D5D8B01A87}" destId="{77618643-8909-4B96-B865-0D76F6C6AC5C}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{D22151FF-90F3-4064-AF05-2D331A6447FF}" type="presOf" srcId="{0D581458-B5EE-4A7F-90FD-3F9112FA4B78}" destId="{2928310D-2CA9-4834-90E6-7BDF49776789}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{AD493D86-C543-4015-BE87-29F68962786B}" type="presOf" srcId="{862D7E0D-F0D4-41D7-97A9-5B92A6FAF196}" destId="{B4A89E68-830E-49C7-8936-A684A6D977A9}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{F89E3577-23BC-4092-A78D-6926C637E5D1}" type="presOf" srcId="{F869AEC1-1E83-4EF1-A608-2ED7273BDA79}" destId="{C57A6536-4127-4AA1-8522-04474917B5F5}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{07549231-1028-4839-90EE-ED2D4CFA9008}" srcId="{90625BEE-1CE8-4E94-BD93-26C691FBA331}" destId="{AE8947B9-4DD1-4CBA-876B-A4D5D8B01A87}" srcOrd="4" destOrd="0" parTransId="{89D5F964-69B4-4004-B7D0-88E04A580D4C}" sibTransId="{74E6B8B5-04F1-47B0-B758-FDE2DD2D1E84}"/>
+    <dgm:cxn modelId="{A0DB7B1F-CF71-4EF2-8DF4-231F649ACACD}" type="presOf" srcId="{50773849-F511-4835-AD5C-FC578FA128E4}" destId="{747F2FED-B883-4887-A704-3213D63B59EB}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{80690E98-44DE-474F-96AD-37737EBE6006}" type="presOf" srcId="{862D7E0D-F0D4-41D7-97A9-5B92A6FAF196}" destId="{00785835-E3F4-4EF8-924A-607B1BE17BA3}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{BBBBFC24-5922-4864-9A93-7D550876B03D}" srcId="{90625BEE-1CE8-4E94-BD93-26C691FBA331}" destId="{656B0FA4-A7DA-4D70-9B17-633C6CD7B506}" srcOrd="1" destOrd="0" parTransId="{23DA1795-4ACE-4459-B5FA-3766EB5DF9C5}" sibTransId="{8D6D3067-77F2-44F8-AE5E-4D8FF3F2F5B2}"/>
+    <dgm:cxn modelId="{1FD79E27-935D-44F1-A586-B49C57823F68}" type="presOf" srcId="{89D5F964-69B4-4004-B7D0-88E04A580D4C}" destId="{993DFE86-1DCA-48E6-AB6D-7101F7F884D6}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{E32E1CDD-73E3-42B3-A0EA-B3D9D6F682C3}" type="presOf" srcId="{B56F1F7B-9CAF-4E3C-8845-E5A0D88E4AC1}" destId="{FFF9F715-5053-4613-89FA-1E0570F1C0C0}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{0F9AB5E7-E337-4889-AB7C-6F392B74B41B}" type="presOf" srcId="{237A5FB3-0392-40DF-98C3-051D76C85975}" destId="{F4C3505A-509D-492B-A76D-03D866D48A9B}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{FC46046D-CE9D-4FB8-9DC6-2EA1C1776976}" type="presOf" srcId="{656B0FA4-A7DA-4D70-9B17-633C6CD7B506}" destId="{638ED046-8A50-4647-BF8C-DC993BB3E9B8}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
     <dgm:cxn modelId="{CD61DB0A-B629-49DD-B878-4C06AA3A3AE8}" srcId="{90625BEE-1CE8-4E94-BD93-26C691FBA331}" destId="{F869AEC1-1E83-4EF1-A608-2ED7273BDA79}" srcOrd="0" destOrd="0" parTransId="{C1626232-3005-446D-A578-0D8DD393590B}" sibTransId="{6452D633-FE9F-435E-9089-7302FF61B0B4}"/>
-    <dgm:cxn modelId="{F89E3577-23BC-4092-A78D-6926C637E5D1}" type="presOf" srcId="{F869AEC1-1E83-4EF1-A608-2ED7273BDA79}" destId="{C57A6536-4127-4AA1-8522-04474917B5F5}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{5C199323-C776-407F-B4A7-96CE1F728BFC}" type="presOf" srcId="{AE8947B9-4DD1-4CBA-876B-A4D5D8B01A87}" destId="{82DF419B-8EE6-4CB7-BAB1-86FC9D1E9AC1}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{9B39BB91-BCA2-4F88-A888-A93460ACAC0D}" srcId="{656B0FA4-A7DA-4D70-9B17-633C6CD7B506}" destId="{A6185CF1-A6C9-4057-B034-F738C98E78D8}" srcOrd="0" destOrd="0" parTransId="{4FB2B5CC-B5E8-4444-9946-1293B3748920}" sibTransId="{E6879C87-8E8C-49ED-9950-ECD513F23E89}"/>
+    <dgm:cxn modelId="{1974D637-A2B6-4A9D-835D-F75A876943E7}" type="presOf" srcId="{23DA1795-4ACE-4459-B5FA-3766EB5DF9C5}" destId="{8B733281-3DE3-4C42-A883-193A9A249CD6}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
     <dgm:cxn modelId="{21BE257A-D0D0-4391-BE49-CB8903F75F88}" srcId="{90625BEE-1CE8-4E94-BD93-26C691FBA331}" destId="{50773849-F511-4835-AD5C-FC578FA128E4}" srcOrd="2" destOrd="0" parTransId="{194D08C5-57EB-4155-B6F2-C4119AFD4E36}" sibTransId="{153384F9-AE57-4070-8EA4-71D24C7CF196}"/>
-    <dgm:cxn modelId="{D22151FF-90F3-4064-AF05-2D331A6447FF}" type="presOf" srcId="{0D581458-B5EE-4A7F-90FD-3F9112FA4B78}" destId="{2928310D-2CA9-4834-90E6-7BDF49776789}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{A0DB7B1F-CF71-4EF2-8DF4-231F649ACACD}" type="presOf" srcId="{50773849-F511-4835-AD5C-FC578FA128E4}" destId="{747F2FED-B883-4887-A704-3213D63B59EB}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{5B2F66D6-2E7D-4412-81A9-A3C99C3D835D}" type="presOf" srcId="{4FB2B5CC-B5E8-4444-9946-1293B3748920}" destId="{CCD8050B-E3A1-4D78-A2EC-AF861030206E}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
     <dgm:cxn modelId="{DCBE64CE-AD06-4484-A607-7AE8805AA703}" type="presOf" srcId="{50773849-F511-4835-AD5C-FC578FA128E4}" destId="{D09303C9-BCC6-4DD2-8E33-C0F1AE38C831}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{E32E1CDD-73E3-42B3-A0EA-B3D9D6F682C3}" type="presOf" srcId="{B56F1F7B-9CAF-4E3C-8845-E5A0D88E4AC1}" destId="{FFF9F715-5053-4613-89FA-1E0570F1C0C0}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{DD52EC3C-F2CD-484A-9560-578DFDD6F601}" type="presOf" srcId="{B56F1F7B-9CAF-4E3C-8845-E5A0D88E4AC1}" destId="{C9C249D0-F1D4-4554-A386-CAFA14270C36}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{63E4C16F-DAFF-4115-824D-4E5062F2889B}" type="presOf" srcId="{90625BEE-1CE8-4E94-BD93-26C691FBA331}" destId="{0508117B-3BAB-41D1-94DF-0CF04275C7FA}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{FC46046D-CE9D-4FB8-9DC6-2EA1C1776976}" type="presOf" srcId="{656B0FA4-A7DA-4D70-9B17-633C6CD7B506}" destId="{638ED046-8A50-4647-BF8C-DC993BB3E9B8}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{B64F773A-90DB-49B8-A18F-5E4035FFF432}" srcId="{0D581458-B5EE-4A7F-90FD-3F9112FA4B78}" destId="{90625BEE-1CE8-4E94-BD93-26C691FBA331}" srcOrd="0" destOrd="0" parTransId="{0F3A10AD-3B79-4301-B641-B9A7875FF524}" sibTransId="{9544EE45-59CE-4B8F-A53E-FCC70B170D25}"/>
-    <dgm:cxn modelId="{71E0349D-088D-4E65-A8C6-D6879D89E856}" type="presOf" srcId="{03BF1FA9-C075-4FA8-BD05-B802322534A6}" destId="{F2B1825C-8BC8-4111-A2C0-A0FBB338DE48}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{1974D637-A2B6-4A9D-835D-F75A876943E7}" type="presOf" srcId="{23DA1795-4ACE-4459-B5FA-3766EB5DF9C5}" destId="{8B733281-3DE3-4C42-A883-193A9A249CD6}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{A02A8C92-53D2-400A-8E31-C1D36C74C310}" type="presOf" srcId="{A6185CF1-A6C9-4057-B034-F738C98E78D8}" destId="{488D30EC-5368-42BE-91A5-E867C0D7A783}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{9B39BB91-BCA2-4F88-A888-A93460ACAC0D}" srcId="{656B0FA4-A7DA-4D70-9B17-633C6CD7B506}" destId="{A6185CF1-A6C9-4057-B034-F738C98E78D8}" srcOrd="0" destOrd="0" parTransId="{4FB2B5CC-B5E8-4444-9946-1293B3748920}" sibTransId="{E6879C87-8E8C-49ED-9950-ECD513F23E89}"/>
-    <dgm:cxn modelId="{325DAB41-614B-4868-B08A-5032FB3CA0F3}" srcId="{50773849-F511-4835-AD5C-FC578FA128E4}" destId="{B56F1F7B-9CAF-4E3C-8845-E5A0D88E4AC1}" srcOrd="0" destOrd="0" parTransId="{237A5FB3-0392-40DF-98C3-051D76C85975}" sibTransId="{D9AC3E19-03F8-4B24-9C05-1F58DDABFDD4}"/>
-    <dgm:cxn modelId="{AD493D86-C543-4015-BE87-29F68962786B}" type="presOf" srcId="{862D7E0D-F0D4-41D7-97A9-5B92A6FAF196}" destId="{B4A89E68-830E-49C7-8936-A684A6D977A9}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{B0173BF3-1663-4869-9510-FF3E6ECDB80B}" type="presOf" srcId="{90625BEE-1CE8-4E94-BD93-26C691FBA331}" destId="{96CAB6C0-43D1-4509-B5E4-801A2235C3C0}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{58D39FB8-3B72-436D-B378-75D5CFD0C8F7}" srcId="{90625BEE-1CE8-4E94-BD93-26C691FBA331}" destId="{862D7E0D-F0D4-41D7-97A9-5B92A6FAF196}" srcOrd="3" destOrd="0" parTransId="{03BF1FA9-C075-4FA8-BD05-B802322534A6}" sibTransId="{C266CAE2-4D1C-4F15-A627-AE1D114514FC}"/>
-    <dgm:cxn modelId="{BBBBFC24-5922-4864-9A93-7D550876B03D}" srcId="{90625BEE-1CE8-4E94-BD93-26C691FBA331}" destId="{656B0FA4-A7DA-4D70-9B17-633C6CD7B506}" srcOrd="1" destOrd="0" parTransId="{23DA1795-4ACE-4459-B5FA-3766EB5DF9C5}" sibTransId="{8D6D3067-77F2-44F8-AE5E-4D8FF3F2F5B2}"/>
-    <dgm:cxn modelId="{1DD651EF-393A-4ECA-BDA5-58D00B75F246}" type="presOf" srcId="{194D08C5-57EB-4155-B6F2-C4119AFD4E36}" destId="{2E25BBEA-DA4E-4795-AB2E-4E623A9015ED}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{C56E1D74-B152-4B9F-8564-CBCE6D400DF6}" type="presOf" srcId="{A6185CF1-A6C9-4057-B034-F738C98E78D8}" destId="{32A9C23E-AD8C-4291-91FD-D6B43BE6B459}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{02C98010-6CFF-47EB-983D-ABB138E78C3F}" type="presOf" srcId="{C1626232-3005-446D-A578-0D8DD393590B}" destId="{D696FE8C-BF81-4065-B3CB-3252DA3B830C}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{0571FFFF-892A-4489-BC21-50013D5FAFB8}" type="presOf" srcId="{656B0FA4-A7DA-4D70-9B17-633C6CD7B506}" destId="{BE5A54D6-F6AF-424F-9423-F66B0C5B6243}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{0F9AB5E7-E337-4889-AB7C-6F392B74B41B}" type="presOf" srcId="{237A5FB3-0392-40DF-98C3-051D76C85975}" destId="{F4C3505A-509D-492B-A76D-03D866D48A9B}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{8BE19EC5-B58E-4BB9-94F6-ED249D783BE0}" type="presOf" srcId="{F869AEC1-1E83-4EF1-A608-2ED7273BDA79}" destId="{E326ADC5-C67D-47B5-8B70-410250FC4F45}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{80690E98-44DE-474F-96AD-37737EBE6006}" type="presOf" srcId="{862D7E0D-F0D4-41D7-97A9-5B92A6FAF196}" destId="{00785835-E3F4-4EF8-924A-607B1BE17BA3}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{5B2F66D6-2E7D-4412-81A9-A3C99C3D835D}" type="presOf" srcId="{4FB2B5CC-B5E8-4444-9946-1293B3748920}" destId="{CCD8050B-E3A1-4D78-A2EC-AF861030206E}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
     <dgm:cxn modelId="{546EAD4A-7D6C-4C9E-8694-592BA2714166}" type="presParOf" srcId="{2928310D-2CA9-4834-90E6-7BDF49776789}" destId="{B2DCFB66-D7FB-48ED-BCA0-9F369E1668C2}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
     <dgm:cxn modelId="{1B4AF8C2-0FBB-4AB5-AB2E-2CD5CDD6F28E}" type="presParOf" srcId="{B2DCFB66-D7FB-48ED-BCA0-9F369E1668C2}" destId="{EAC19A42-ACBD-4DEC-9558-1A920DBAF4EA}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
     <dgm:cxn modelId="{A910809D-AC77-42E6-B902-1CEB623229D4}" type="presParOf" srcId="{EAC19A42-ACBD-4DEC-9558-1A920DBAF4EA}" destId="{0508117B-3BAB-41D1-94DF-0CF04275C7FA}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
@@ -1603,6 +1814,13 @@
     <dgm:cxn modelId="{6B165584-36BD-4F14-A1DD-F887AA717CB4}" type="presParOf" srcId="{1C50B8F7-B0D8-4AC7-9697-96D6DC8A6695}" destId="{00785835-E3F4-4EF8-924A-607B1BE17BA3}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
     <dgm:cxn modelId="{1214E1F8-BE82-47BD-9B57-E21CEC3E3534}" type="presParOf" srcId="{2F6718CB-1A8A-4650-AB72-E9A1BE671FFE}" destId="{7CDF85EA-A31C-46FE-AC6A-AA3C59759A2A}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
     <dgm:cxn modelId="{85EAA32D-1F66-4DFE-8DFD-930DE628AAF1}" type="presParOf" srcId="{2F6718CB-1A8A-4650-AB72-E9A1BE671FFE}" destId="{2004B03C-06A2-4E4D-ABF4-8B17432697AE}" srcOrd="2" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{7E619409-E810-4B94-9726-36F417EDAAA3}" type="presParOf" srcId="{E11E15A6-B9E1-4464-ACAB-B8B240A9A4D9}" destId="{993DFE86-1DCA-48E6-AB6D-7101F7F884D6}" srcOrd="8" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{4A6C3A12-7818-4767-8BCD-23A6D5C3FFCD}" type="presParOf" srcId="{E11E15A6-B9E1-4464-ACAB-B8B240A9A4D9}" destId="{C8B37CB4-59A5-4030-AA67-752675154247}" srcOrd="9" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{EADF4AAA-A6C7-40A8-A7AF-96C1F0892DDB}" type="presParOf" srcId="{C8B37CB4-59A5-4030-AA67-752675154247}" destId="{17CD3FE5-42A0-4E0F-9D5C-426B3CBDC113}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{FD70EEB9-2FC1-4155-9E92-4180E755B200}" type="presParOf" srcId="{17CD3FE5-42A0-4E0F-9D5C-426B3CBDC113}" destId="{77618643-8909-4B96-B865-0D76F6C6AC5C}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{FABA95E2-1CA3-4D53-83A8-2E553398CE7E}" type="presParOf" srcId="{17CD3FE5-42A0-4E0F-9D5C-426B3CBDC113}" destId="{82DF419B-8EE6-4CB7-BAB1-86FC9D1E9AC1}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{89C005EE-1800-4A64-8750-DC1351346520}" type="presParOf" srcId="{C8B37CB4-59A5-4030-AA67-752675154247}" destId="{AB06BFB8-3302-441D-AE77-152478D7B0A2}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{7E48B768-3602-467E-80D7-17E6D2696309}" type="presParOf" srcId="{C8B37CB4-59A5-4030-AA67-752675154247}" destId="{7652BEC3-3C8D-48EA-9EA3-3C49EBEB8780}" srcOrd="2" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
     <dgm:cxn modelId="{520AB15E-990E-4224-B7BB-933DDE923F89}" type="presParOf" srcId="{B2DCFB66-D7FB-48ED-BCA0-9F369E1668C2}" destId="{62033BBF-FDB7-402B-8DA8-A036D51728D0}" srcOrd="2" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
   </dgm:cxnLst>
   <dgm:bg/>
@@ -1623,15 +1841,15 @@
       <dsp:cNvGrpSpPr/>
     </dsp:nvGrpSpPr>
     <dsp:grpSpPr/>
-    <dsp:sp modelId="{F2B1825C-8BC8-4111-A2C0-A0FBB338DE48}">
+    <dsp:sp modelId="{993DFE86-1DCA-48E6-AB6D-7101F7F884D6}">
       <dsp:nvSpPr>
         <dsp:cNvPr id="0" name=""/>
         <dsp:cNvSpPr/>
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="2286000" y="2632332"/>
-          <a:ext cx="1790409" cy="207154"/>
+          <a:off x="2605087" y="2256679"/>
+          <a:ext cx="2158641" cy="187320"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -1645,13 +1863,74 @@
                 <a:pt x="0" y="0"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="0" y="103577"/>
+                <a:pt x="0" y="93660"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="1790409" y="103577"/>
+                <a:pt x="2158641" y="93660"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="1790409" y="207154"/>
+                <a:pt x="2158641" y="187320"/>
+              </a:lnTo>
+            </a:path>
+          </a:pathLst>
+        </a:custGeom>
+        <a:noFill/>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="accent1">
+              <a:shade val="60000"/>
+              <a:hueOff val="0"/>
+              <a:satOff val="0"/>
+              <a:lumOff val="0"/>
+              <a:alphaOff val="0"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:effectLst/>
+      </dsp:spPr>
+      <dsp:style>
+        <a:lnRef idx="2">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor"/>
+      </dsp:style>
+    </dsp:sp>
+    <dsp:sp modelId="{F2B1825C-8BC8-4111-A2C0-A0FBB338DE48}">
+      <dsp:nvSpPr>
+        <dsp:cNvPr id="0" name=""/>
+        <dsp:cNvSpPr/>
+      </dsp:nvSpPr>
+      <dsp:spPr>
+        <a:xfrm>
+          <a:off x="2605087" y="2256679"/>
+          <a:ext cx="1079320" cy="187320"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst>
+            <a:path>
+              <a:moveTo>
+                <a:pt x="0" y="0"/>
+              </a:moveTo>
+              <a:lnTo>
+                <a:pt x="0" y="93660"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="1079320" y="93660"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="1079320" y="187320"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -1691,8 +1970,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="2488222" y="3332712"/>
-          <a:ext cx="147967" cy="453767"/>
+          <a:off x="2248287" y="2890000"/>
+          <a:ext cx="133800" cy="410320"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -1706,10 +1985,10 @@
                 <a:pt x="0" y="0"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="0" y="453767"/>
+                <a:pt x="0" y="410320"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="147967" y="453767"/>
+                <a:pt x="133800" y="410320"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -1749,8 +2028,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="2286000" y="2632332"/>
-          <a:ext cx="596803" cy="207154"/>
+          <a:off x="2559367" y="2256679"/>
+          <a:ext cx="91440" cy="187320"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -1761,16 +2040,10 @@
           <a:pathLst>
             <a:path>
               <a:moveTo>
-                <a:pt x="0" y="0"/>
+                <a:pt x="45720" y="0"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="0" y="103577"/>
-              </a:lnTo>
-              <a:lnTo>
-                <a:pt x="596803" y="103577"/>
-              </a:lnTo>
-              <a:lnTo>
-                <a:pt x="596803" y="207154"/>
+                <a:pt x="45720" y="187320"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -1810,8 +2083,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="1294616" y="3332712"/>
-          <a:ext cx="147967" cy="453767"/>
+          <a:off x="1168966" y="2890000"/>
+          <a:ext cx="133800" cy="410320"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -1825,10 +2098,10 @@
                 <a:pt x="0" y="0"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="0" y="453767"/>
+                <a:pt x="0" y="410320"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="147967" y="453767"/>
+                <a:pt x="133800" y="410320"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -1868,8 +2141,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="1689196" y="2632332"/>
-          <a:ext cx="596803" cy="207154"/>
+          <a:off x="1525766" y="2256679"/>
+          <a:ext cx="1079320" cy="187320"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -1880,16 +2153,16 @@
           <a:pathLst>
             <a:path>
               <a:moveTo>
-                <a:pt x="596803" y="0"/>
+                <a:pt x="1079320" y="0"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="596803" y="103577"/>
+                <a:pt x="1079320" y="93660"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="0" y="103577"/>
+                <a:pt x="0" y="93660"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="0" y="207154"/>
+                <a:pt x="0" y="187320"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -1929,8 +2202,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="495590" y="2632332"/>
-          <a:ext cx="1790409" cy="207154"/>
+          <a:off x="446445" y="2256679"/>
+          <a:ext cx="2158641" cy="187320"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -1941,16 +2214,16 @@
           <a:pathLst>
             <a:path>
               <a:moveTo>
-                <a:pt x="1790409" y="0"/>
+                <a:pt x="2158641" y="0"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="1790409" y="103577"/>
+                <a:pt x="2158641" y="93660"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="0" y="103577"/>
+                <a:pt x="0" y="93660"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="0" y="207154"/>
+                <a:pt x="0" y="187320"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -1990,8 +2263,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="1792774" y="2139106"/>
-          <a:ext cx="986451" cy="493225"/>
+          <a:off x="2159087" y="1810679"/>
+          <a:ext cx="892000" cy="446000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2032,12 +2305,12 @@
         </a:fontRef>
       </dsp:style>
       <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="6350" tIns="6350" rIns="6350" bIns="6350" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="5715" tIns="5715" rIns="5715" bIns="5715" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
           <a:noAutofit/>
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr lvl="0" algn="ctr" defTabSz="444500">
+          <a:pPr lvl="0" algn="ctr" defTabSz="400050">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -2049,14 +2322,14 @@
             </a:spcAft>
           </a:pPr>
           <a:r>
-            <a:rPr lang="pl-PL" sz="1000" kern="1200"/>
+            <a:rPr lang="pl-PL" sz="900" kern="1200"/>
             <a:t>User</a:t>
           </a:r>
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="1792774" y="2139106"/>
-        <a:ext cx="986451" cy="493225"/>
+        <a:off x="2159087" y="1810679"/>
+        <a:ext cx="892000" cy="446000"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{C57A6536-4127-4AA1-8522-04474917B5F5}">
@@ -2066,8 +2339,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="2364" y="2839487"/>
-          <a:ext cx="986451" cy="493225"/>
+          <a:off x="445" y="2443999"/>
+          <a:ext cx="892000" cy="446000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2108,12 +2381,12 @@
         </a:fontRef>
       </dsp:style>
       <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="6350" tIns="6350" rIns="6350" bIns="6350" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="5715" tIns="5715" rIns="5715" bIns="5715" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
           <a:noAutofit/>
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr lvl="0" algn="ctr" defTabSz="444500">
+          <a:pPr lvl="0" algn="ctr" defTabSz="400050">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -2125,14 +2398,14 @@
             </a:spcAft>
           </a:pPr>
           <a:r>
-            <a:rPr lang="pl-PL" sz="1000" kern="1200"/>
+            <a:rPr lang="pl-PL" sz="900" kern="1200"/>
             <a:t>user_details</a:t>
           </a:r>
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="2364" y="2839487"/>
-        <a:ext cx="986451" cy="493225"/>
+        <a:off x="445" y="2443999"/>
+        <a:ext cx="892000" cy="446000"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{638ED046-8A50-4647-BF8C-DC993BB3E9B8}">
@@ -2142,8 +2415,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="1195971" y="2839487"/>
-          <a:ext cx="986451" cy="493225"/>
+          <a:off x="1079766" y="2443999"/>
+          <a:ext cx="892000" cy="446000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2184,12 +2457,12 @@
         </a:fontRef>
       </dsp:style>
       <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="6350" tIns="6350" rIns="6350" bIns="6350" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="5715" tIns="5715" rIns="5715" bIns="5715" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
           <a:noAutofit/>
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr lvl="0" algn="ctr" defTabSz="444500">
+          <a:pPr lvl="0" algn="ctr" defTabSz="400050">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -2201,14 +2474,14 @@
             </a:spcAft>
           </a:pPr>
           <a:r>
-            <a:rPr lang="pl-PL" sz="1000" kern="1200"/>
+            <a:rPr lang="pl-PL" sz="900" kern="1200"/>
             <a:t>user_shopping_list</a:t>
           </a:r>
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="1195971" y="2839487"/>
-        <a:ext cx="986451" cy="493225"/>
+        <a:off x="1079766" y="2443999"/>
+        <a:ext cx="892000" cy="446000"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{488D30EC-5368-42BE-91A5-E867C0D7A783}">
@@ -2218,8 +2491,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="1442584" y="3539867"/>
-          <a:ext cx="986451" cy="493225"/>
+          <a:off x="1302766" y="3077320"/>
+          <a:ext cx="892000" cy="446000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2260,12 +2533,12 @@
         </a:fontRef>
       </dsp:style>
       <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="6350" tIns="6350" rIns="6350" bIns="6350" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="5715" tIns="5715" rIns="5715" bIns="5715" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
           <a:noAutofit/>
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr lvl="0" algn="ctr" defTabSz="444500">
+          <a:pPr lvl="0" algn="ctr" defTabSz="400050">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -2277,14 +2550,14 @@
             </a:spcAft>
           </a:pPr>
           <a:r>
-            <a:rPr lang="pl-PL" sz="1000" kern="1200"/>
+            <a:rPr lang="pl-PL" sz="900" kern="1200"/>
             <a:t>shopping_list</a:t>
           </a:r>
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="1442584" y="3539867"/>
-        <a:ext cx="986451" cy="493225"/>
+        <a:off x="1302766" y="3077320"/>
+        <a:ext cx="892000" cy="446000"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{747F2FED-B883-4887-A704-3213D63B59EB}">
@@ -2294,8 +2567,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="2389577" y="2839487"/>
-          <a:ext cx="986451" cy="493225"/>
+          <a:off x="2159087" y="2443999"/>
+          <a:ext cx="892000" cy="446000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2336,12 +2609,12 @@
         </a:fontRef>
       </dsp:style>
       <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="6350" tIns="6350" rIns="6350" bIns="6350" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="5715" tIns="5715" rIns="5715" bIns="5715" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
           <a:noAutofit/>
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr lvl="0" algn="ctr" defTabSz="444500">
+          <a:pPr lvl="0" algn="ctr" defTabSz="400050">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -2353,14 +2626,14 @@
             </a:spcAft>
           </a:pPr>
           <a:r>
-            <a:rPr lang="pl-PL" sz="1000" kern="1200"/>
+            <a:rPr lang="pl-PL" sz="900" kern="1200"/>
             <a:t>user_med_tests</a:t>
           </a:r>
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="2389577" y="2839487"/>
-        <a:ext cx="986451" cy="493225"/>
+        <a:off x="2159087" y="2443999"/>
+        <a:ext cx="892000" cy="446000"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{C9C249D0-F1D4-4554-A386-CAFA14270C36}">
@@ -2370,8 +2643,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="2636190" y="3539867"/>
-          <a:ext cx="986451" cy="493225"/>
+          <a:off x="2382087" y="3077320"/>
+          <a:ext cx="892000" cy="446000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2412,12 +2685,12 @@
         </a:fontRef>
       </dsp:style>
       <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="6350" tIns="6350" rIns="6350" bIns="6350" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="5715" tIns="5715" rIns="5715" bIns="5715" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
           <a:noAutofit/>
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr lvl="0" algn="ctr" defTabSz="444500">
+          <a:pPr lvl="0" algn="ctr" defTabSz="400050">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -2429,14 +2702,14 @@
             </a:spcAft>
           </a:pPr>
           <a:r>
-            <a:rPr lang="pl-PL" sz="1000" kern="1200"/>
+            <a:rPr lang="pl-PL" sz="900" kern="1200"/>
             <a:t>med_tests</a:t>
           </a:r>
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="2636190" y="3539867"/>
-        <a:ext cx="986451" cy="493225"/>
+        <a:off x="2382087" y="3077320"/>
+        <a:ext cx="892000" cy="446000"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{B4A89E68-830E-49C7-8936-A684A6D977A9}">
@@ -2446,8 +2719,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="3583183" y="2839487"/>
-          <a:ext cx="986451" cy="493225"/>
+          <a:off x="3238408" y="2443999"/>
+          <a:ext cx="892000" cy="446000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2488,12 +2761,12 @@
         </a:fontRef>
       </dsp:style>
       <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="6350" tIns="6350" rIns="6350" bIns="6350" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="5715" tIns="5715" rIns="5715" bIns="5715" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
           <a:noAutofit/>
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr lvl="0" algn="ctr" defTabSz="444500">
+          <a:pPr lvl="0" algn="ctr" defTabSz="400050">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -2505,14 +2778,90 @@
             </a:spcAft>
           </a:pPr>
           <a:r>
-            <a:rPr lang="pl-PL" sz="1000" kern="1200"/>
+            <a:rPr lang="pl-PL" sz="900" kern="1200"/>
             <a:t>pregnacy</a:t>
           </a:r>
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="3583183" y="2839487"/>
-        <a:ext cx="986451" cy="493225"/>
+        <a:off x="3238408" y="2443999"/>
+        <a:ext cx="892000" cy="446000"/>
+      </dsp:txXfrm>
+    </dsp:sp>
+    <dsp:sp modelId="{77618643-8909-4B96-B865-0D76F6C6AC5C}">
+      <dsp:nvSpPr>
+        <dsp:cNvPr id="0" name=""/>
+        <dsp:cNvSpPr/>
+      </dsp:nvSpPr>
+      <dsp:spPr>
+        <a:xfrm>
+          <a:off x="4317729" y="2443999"/>
+          <a:ext cx="892000" cy="446000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent1">
+            <a:hueOff val="0"/>
+            <a:satOff val="0"/>
+            <a:lumOff val="0"/>
+            <a:alphaOff val="0"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:hueOff val="0"/>
+              <a:satOff val="0"/>
+              <a:lumOff val="0"/>
+              <a:alphaOff val="0"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:effectLst/>
+      </dsp:spPr>
+      <dsp:style>
+        <a:lnRef idx="2">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </dsp:style>
+      <dsp:txBody>
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="5715" tIns="5715" rIns="5715" bIns="5715" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr lvl="0" algn="ctr" defTabSz="400050">
+            <a:lnSpc>
+              <a:spcPct val="90000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPct val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPct val="35000"/>
+            </a:spcAft>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="pl-PL" sz="900" kern="1200"/>
+            <a:t>passwds</a:t>
+          </a:r>
+        </a:p>
+      </dsp:txBody>
+      <dsp:txXfrm>
+        <a:off x="4317729" y="2443999"/>
+        <a:ext cx="892000" cy="446000"/>
       </dsp:txXfrm>
     </dsp:sp>
   </dsp:spTree>
@@ -4703,16 +5052,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>66675</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>371475</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5019,10 +5368,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G36"/>
+  <dimension ref="A1:G39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5040,13 +5389,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>11</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
@@ -5057,62 +5406,89 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
         <v>12</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>13</v>
       </c>
-      <c r="D2" t="s">
-        <v>14</v>
-      </c>
       <c r="E2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="B3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="B4" t="s">
-        <v>16</v>
+        <v>46</v>
+      </c>
+      <c r="C4" t="s">
+        <v>47</v>
+      </c>
+      <c r="E4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:7">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="B6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" t="s">
+        <v>25</v>
+      </c>
+      <c r="F6" t="s">
         <v>18</v>
+      </c>
+      <c r="G6" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" t="s">
-        <v>2</v>
-      </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>44</v>
       </c>
       <c r="C7" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" t="s">
-        <v>14</v>
+        <v>42</v>
       </c>
       <c r="E7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -5120,336 +5496,381 @@
         <v>15</v>
       </c>
       <c r="C8" t="s">
-        <v>21</v>
+        <v>45</v>
       </c>
       <c r="E8" t="s">
-        <v>26</v>
-      </c>
-      <c r="F8" t="s">
-        <v>19</v>
-      </c>
-      <c r="G8" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="B9" t="s">
-        <v>48</v>
+        <v>16</v>
       </c>
       <c r="C9" t="s">
-        <v>4</v>
+        <v>34</v>
       </c>
       <c r="E9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:7">
-      <c r="A10" t="s">
-        <v>3</v>
-      </c>
       <c r="B10" t="s">
-        <v>4</v>
+        <v>17</v>
+      </c>
+      <c r="C10" t="s">
+        <v>42</v>
+      </c>
+      <c r="E10" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" t="s">
         <v>12</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>13</v>
       </c>
-      <c r="D11" t="s">
-        <v>14</v>
-      </c>
       <c r="E11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="B12" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="C12" t="s">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="E12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F12" t="s">
-        <v>19</v>
+        <v>18</v>
+      </c>
+      <c r="G12" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:7">
       <c r="B13" t="s">
-        <v>28</v>
+        <v>49</v>
       </c>
       <c r="C13" t="s">
-        <v>13</v>
+        <v>50</v>
       </c>
       <c r="E13" t="s">
-        <v>26</v>
+        <v>25</v>
+      </c>
+      <c r="F13" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:7">
+      <c r="A14" t="s">
+        <v>4</v>
+      </c>
       <c r="B14" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="C14" t="s">
+        <v>12</v>
+      </c>
+      <c r="D14" t="s">
         <v>13</v>
+      </c>
+      <c r="E14" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="15" spans="1:7">
       <c r="B15" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C15" t="s">
-        <v>4</v>
+        <v>34</v>
+      </c>
+      <c r="E15" t="s">
+        <v>25</v>
+      </c>
+      <c r="F15" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c r="B16" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C16" t="s">
-        <v>36</v>
+        <v>12</v>
       </c>
       <c r="E16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="17" spans="1:7">
       <c r="B17" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C17" t="s">
-        <v>36</v>
+        <v>12</v>
       </c>
     </row>
     <row r="18" spans="1:7">
-      <c r="A18" t="s">
-        <v>6</v>
-      </c>
       <c r="B18" t="s">
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="C18" t="s">
-        <v>13</v>
-      </c>
-      <c r="D18" t="s">
-        <v>14</v>
-      </c>
-      <c r="E18" t="s">
-        <v>26</v>
+        <v>51</v>
       </c>
     </row>
     <row r="19" spans="1:7">
       <c r="B19" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="C19" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="E19" t="s">
-        <v>26</v>
-      </c>
-      <c r="F19" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
     </row>
     <row r="20" spans="1:7">
       <c r="B20" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="C20" t="s">
-        <v>41</v>
-      </c>
-      <c r="E20" t="s">
-        <v>26</v>
+        <v>48</v>
       </c>
     </row>
     <row r="21" spans="1:7">
+      <c r="A21" t="s">
+        <v>5</v>
+      </c>
       <c r="B21" t="s">
-        <v>39</v>
+        <v>11</v>
       </c>
       <c r="C21" t="s">
-        <v>41</v>
+        <v>12</v>
+      </c>
+      <c r="D21" t="s">
+        <v>13</v>
+      </c>
+      <c r="E21" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="22" spans="1:7">
       <c r="B22" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C22" t="s">
-        <v>43</v>
+        <v>39</v>
+      </c>
+      <c r="E22" t="s">
+        <v>25</v>
+      </c>
+      <c r="F22" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="23" spans="1:7">
       <c r="B23" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="C23" t="s">
-        <v>36</v>
+        <v>39</v>
+      </c>
+      <c r="E23" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="24" spans="1:7">
       <c r="B24" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="C24" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
     <row r="25" spans="1:7">
-      <c r="A25" t="s">
-        <v>7</v>
-      </c>
       <c r="B25" t="s">
-        <v>12</v>
+        <v>38</v>
       </c>
       <c r="C25" t="s">
-        <v>13</v>
-      </c>
-      <c r="D25" t="s">
-        <v>14</v>
-      </c>
-      <c r="E25" t="s">
-        <v>26</v>
+        <v>48</v>
       </c>
     </row>
     <row r="26" spans="1:7">
       <c r="B26" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="C26" t="s">
-        <v>35</v>
-      </c>
-      <c r="E26" t="s">
-        <v>26</v>
-      </c>
-      <c r="F26" t="s">
-        <v>19</v>
-      </c>
-      <c r="G26" t="s">
-        <v>37</v>
+        <v>48</v>
       </c>
     </row>
     <row r="27" spans="1:7">
       <c r="B27" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C27" t="s">
-        <v>13</v>
+        <v>48</v>
       </c>
     </row>
     <row r="28" spans="1:7">
+      <c r="A28" t="s">
+        <v>6</v>
+      </c>
       <c r="B28" t="s">
-        <v>34</v>
+        <v>11</v>
       </c>
       <c r="C28" t="s">
-        <v>36</v>
+        <v>12</v>
+      </c>
+      <c r="D28" t="s">
+        <v>13</v>
+      </c>
+      <c r="E28" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="29" spans="1:7">
-      <c r="A29" t="s">
-        <v>8</v>
-      </c>
       <c r="B29" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="C29" t="s">
-        <v>13</v>
-      </c>
-      <c r="D29" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="E29" t="s">
-        <v>26</v>
+        <v>25</v>
+      </c>
+      <c r="F29" t="s">
+        <v>18</v>
+      </c>
+      <c r="G29" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="30" spans="1:7">
       <c r="B30" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C30" t="s">
-        <v>41</v>
-      </c>
-      <c r="E30" t="s">
-        <v>26</v>
-      </c>
-      <c r="F30" t="s">
-        <v>19</v>
-      </c>
-      <c r="G30" t="s">
-        <v>47</v>
+        <v>12</v>
       </c>
     </row>
     <row r="31" spans="1:7">
       <c r="B31" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="C31" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="32" spans="1:7">
+      <c r="A32" t="s">
+        <v>7</v>
+      </c>
       <c r="B32" t="s">
-        <v>45</v>
+        <v>11</v>
       </c>
       <c r="C32" t="s">
-        <v>4</v>
+        <v>12</v>
+      </c>
+      <c r="D32" t="s">
+        <v>13</v>
+      </c>
+      <c r="E32" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="33" spans="1:7">
       <c r="B33" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C33" t="s">
-        <v>36</v>
+        <v>39</v>
+      </c>
+      <c r="E33" t="s">
+        <v>25</v>
+      </c>
+      <c r="F33" t="s">
+        <v>18</v>
+      </c>
+      <c r="G33" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="34" spans="1:7">
-      <c r="A34" t="s">
-        <v>24</v>
-      </c>
       <c r="B34" t="s">
-        <v>12</v>
+        <v>41</v>
       </c>
       <c r="C34" t="s">
-        <v>13</v>
-      </c>
-      <c r="D34" t="s">
-        <v>14</v>
-      </c>
-      <c r="E34" t="s">
-        <v>26</v>
+        <v>48</v>
       </c>
     </row>
     <row r="35" spans="1:7">
       <c r="B35" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
       <c r="C35" t="s">
-        <v>21</v>
-      </c>
-      <c r="E35" t="s">
-        <v>26</v>
-      </c>
-      <c r="F35" t="s">
-        <v>22</v>
-      </c>
-      <c r="G35" t="s">
-        <v>23</v>
+        <v>42</v>
       </c>
     </row>
     <row r="36" spans="1:7">
       <c r="B36" t="s">
+        <v>33</v>
+      </c>
+      <c r="C36" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7">
+      <c r="A37" t="s">
+        <v>23</v>
+      </c>
+      <c r="B37" t="s">
+        <v>11</v>
+      </c>
+      <c r="C37" t="s">
+        <v>12</v>
+      </c>
+      <c r="D37" t="s">
+        <v>13</v>
+      </c>
+      <c r="E37" t="s">
         <v>25</v>
       </c>
-      <c r="C36" t="s">
-        <v>13</v>
+    </row>
+    <row r="38" spans="1:7">
+      <c r="B38" t="s">
+        <v>19</v>
+      </c>
+      <c r="C38" t="s">
+        <v>20</v>
+      </c>
+      <c r="E38" t="s">
+        <v>25</v>
+      </c>
+      <c r="F38" t="s">
+        <v>21</v>
+      </c>
+      <c r="G38" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7">
+      <c r="B39" t="s">
+        <v>24</v>
+      </c>
+      <c r="C39" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding more queries to db
</commit_message>
<xml_diff>
--- a/assets/doku/DB tables.xlsx
+++ b/assets/doku/DB tables.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="51">
   <si>
     <t>Table</t>
   </si>
@@ -168,9 +168,6 @@
     <t>passwd</t>
   </si>
   <si>
-    <t>varchar(60)</t>
-  </si>
-  <si>
     <t>blob</t>
   </si>
 </sst>
@@ -1682,6 +1679,13 @@
     <dgm:pt modelId="{993DFE86-1DCA-48E6-AB6D-7101F7F884D6}" type="pres">
       <dgm:prSet presAssocID="{89D5F964-69B4-4004-B7D0-88E04A580D4C}" presName="Name37" presStyleLbl="parChTrans1D2" presStyleIdx="4" presStyleCnt="5"/>
       <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="pl-PL"/>
+        </a:p>
+      </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{C8B37CB4-59A5-4030-AA67-752675154247}" type="pres">
       <dgm:prSet presAssocID="{AE8947B9-4DD1-4CBA-876B-A4D5D8B01A87}" presName="hierRoot2" presStyleCnt="0">
@@ -5371,7 +5375,7 @@
   <dimension ref="A1:G39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5568,9 +5572,6 @@
       <c r="E13" t="s">
         <v>25</v>
       </c>
-      <c r="F13" t="s">
-        <v>18</v>
-      </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" t="s">
@@ -5627,7 +5628,7 @@
         <v>29</v>
       </c>
       <c r="C18" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="19" spans="1:7">

</xml_diff>

<commit_message>
Working on storing images in db + prepare backup local image storage solution
</commit_message>
<xml_diff>
--- a/assets/doku/DB tables.xlsx
+++ b/assets/doku/DB tables.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="62">
   <si>
     <t>Table</t>
   </si>
@@ -99,9 +99,6 @@
     <t>item_name</t>
   </si>
   <si>
-    <t>item_price</t>
-  </si>
-  <si>
     <t>recomm_amount</t>
   </si>
   <si>
@@ -169,6 +166,42 @@
   </si>
   <si>
     <t>blob</t>
+  </si>
+  <si>
+    <t>varchar(250)</t>
+  </si>
+  <si>
+    <t>currency</t>
+  </si>
+  <si>
+    <t>varchar(50)</t>
+  </si>
+  <si>
+    <t>double</t>
+  </si>
+  <si>
+    <t>img_src</t>
+  </si>
+  <si>
+    <t>Binary(16)</t>
+  </si>
+  <si>
+    <t>auto_increment</t>
+  </si>
+  <si>
+    <t>longblob</t>
+  </si>
+  <si>
+    <t>INTEGER</t>
+  </si>
+  <si>
+    <t>foreing_key(img_src.id)</t>
+  </si>
+  <si>
+    <t>category</t>
+  </si>
+  <si>
+    <t>item_price_range</t>
   </si>
 </sst>
 </file>
@@ -1272,6 +1305,28 @@
         </a:p>
       </dgm:t>
     </dgm:pt>
+    <dgm:pt modelId="{31984FD3-2923-4172-BF0B-1AD9B9A01FD5}">
+      <dgm:prSet phldrT="[Tekst]"/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="pl-PL"/>
+            <a:t>img_src</a:t>
+          </a:r>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{4E1CD3DD-F8B4-4A0F-97E8-1A1E5C772D18}" type="parTrans" cxnId="{CC4146FF-ADDE-46CB-BD84-61F7CA13E7EC}">
+      <dgm:prSet/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{5F56B929-C765-4B7E-81DE-6F334B61057E}" type="sibTrans" cxnId="{CC4146FF-ADDE-46CB-BD84-61F7CA13E7EC}">
+      <dgm:prSet/>
+      <dgm:spPr/>
+    </dgm:pt>
     <dgm:pt modelId="{2928310D-2CA9-4834-90E6-7BDF49776789}" type="pres">
       <dgm:prSet presAssocID="{0D581458-B5EE-4A7F-90FD-3F9112FA4B78}" presName="hierChild1" presStyleCnt="0">
         <dgm:presLayoutVars>
@@ -1497,16 +1552,28 @@
       <dgm:prSet presAssocID="{A6185CF1-A6C9-4057-B034-F738C98E78D8}" presName="hierChild4" presStyleCnt="0"/>
       <dgm:spPr/>
     </dgm:pt>
-    <dgm:pt modelId="{E7F26332-31D7-4D14-887D-38AC3F6B542D}" type="pres">
-      <dgm:prSet presAssocID="{A6185CF1-A6C9-4057-B034-F738C98E78D8}" presName="hierChild5" presStyleCnt="0"/>
-      <dgm:spPr/>
-    </dgm:pt>
-    <dgm:pt modelId="{5196F5DF-44C1-47A9-A6ED-F4D25A01B422}" type="pres">
-      <dgm:prSet presAssocID="{656B0FA4-A7DA-4D70-9B17-633C6CD7B506}" presName="hierChild5" presStyleCnt="0"/>
-      <dgm:spPr/>
-    </dgm:pt>
-    <dgm:pt modelId="{2E25BBEA-DA4E-4795-AB2E-4E623A9015ED}" type="pres">
-      <dgm:prSet presAssocID="{194D08C5-57EB-4155-B6F2-C4119AFD4E36}" presName="Name37" presStyleLbl="parChTrans1D2" presStyleIdx="2" presStyleCnt="5"/>
+    <dgm:pt modelId="{ACC15529-EE74-465D-8E76-84913ECA718C}" type="pres">
+      <dgm:prSet presAssocID="{4E1CD3DD-F8B4-4A0F-97E8-1A1E5C772D18}" presName="Name37" presStyleLbl="parChTrans1D4" presStyleIdx="0" presStyleCnt="1"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{EB97A818-6508-4738-A451-20FFF43ED8D6}" type="pres">
+      <dgm:prSet presAssocID="{31984FD3-2923-4172-BF0B-1AD9B9A01FD5}" presName="hierRoot2" presStyleCnt="0">
+        <dgm:presLayoutVars>
+          <dgm:hierBranch val="init"/>
+        </dgm:presLayoutVars>
+      </dgm:prSet>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{F4F92C47-4DB4-4F3D-AF9B-3AA6C3E64951}" type="pres">
+      <dgm:prSet presAssocID="{31984FD3-2923-4172-BF0B-1AD9B9A01FD5}" presName="rootComposite" presStyleCnt="0"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{71963852-35F0-42CE-850C-B12317072D70}" type="pres">
+      <dgm:prSet presAssocID="{31984FD3-2923-4172-BF0B-1AD9B9A01FD5}" presName="rootText" presStyleLbl="node4" presStyleIdx="0" presStyleCnt="1">
+        <dgm:presLayoutVars>
+          <dgm:chPref val="3"/>
+        </dgm:presLayoutVars>
+      </dgm:prSet>
       <dgm:spPr/>
       <dgm:t>
         <a:bodyPr/>
@@ -1516,24 +1583,8 @@
         </a:p>
       </dgm:t>
     </dgm:pt>
-    <dgm:pt modelId="{75E405C0-9842-4565-8FB6-DDB1CAFFD11A}" type="pres">
-      <dgm:prSet presAssocID="{50773849-F511-4835-AD5C-FC578FA128E4}" presName="hierRoot2" presStyleCnt="0">
-        <dgm:presLayoutVars>
-          <dgm:hierBranch val="init"/>
-        </dgm:presLayoutVars>
-      </dgm:prSet>
-      <dgm:spPr/>
-    </dgm:pt>
-    <dgm:pt modelId="{C7823C8D-F1A4-41A9-AAC6-90587AC45B04}" type="pres">
-      <dgm:prSet presAssocID="{50773849-F511-4835-AD5C-FC578FA128E4}" presName="rootComposite" presStyleCnt="0"/>
-      <dgm:spPr/>
-    </dgm:pt>
-    <dgm:pt modelId="{747F2FED-B883-4887-A704-3213D63B59EB}" type="pres">
-      <dgm:prSet presAssocID="{50773849-F511-4835-AD5C-FC578FA128E4}" presName="rootText" presStyleLbl="node2" presStyleIdx="2" presStyleCnt="5">
-        <dgm:presLayoutVars>
-          <dgm:chPref val="3"/>
-        </dgm:presLayoutVars>
-      </dgm:prSet>
+    <dgm:pt modelId="{6FC1C387-5713-4261-B66C-02A4F0A263E3}" type="pres">
+      <dgm:prSet presAssocID="{31984FD3-2923-4172-BF0B-1AD9B9A01FD5}" presName="rootConnector" presStyleLbl="node4" presStyleIdx="0" presStyleCnt="1"/>
       <dgm:spPr/>
       <dgm:t>
         <a:bodyPr/>
@@ -1543,8 +1594,24 @@
         </a:p>
       </dgm:t>
     </dgm:pt>
-    <dgm:pt modelId="{D09303C9-BCC6-4DD2-8E33-C0F1AE38C831}" type="pres">
-      <dgm:prSet presAssocID="{50773849-F511-4835-AD5C-FC578FA128E4}" presName="rootConnector" presStyleLbl="node2" presStyleIdx="2" presStyleCnt="5"/>
+    <dgm:pt modelId="{FAEFEE1A-3D8E-455A-B487-F61EB5EA8FE0}" type="pres">
+      <dgm:prSet presAssocID="{31984FD3-2923-4172-BF0B-1AD9B9A01FD5}" presName="hierChild4" presStyleCnt="0"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{279CE8DD-7BE7-47A8-872B-FF55B77EB153}" type="pres">
+      <dgm:prSet presAssocID="{31984FD3-2923-4172-BF0B-1AD9B9A01FD5}" presName="hierChild5" presStyleCnt="0"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{E7F26332-31D7-4D14-887D-38AC3F6B542D}" type="pres">
+      <dgm:prSet presAssocID="{A6185CF1-A6C9-4057-B034-F738C98E78D8}" presName="hierChild5" presStyleCnt="0"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{5196F5DF-44C1-47A9-A6ED-F4D25A01B422}" type="pres">
+      <dgm:prSet presAssocID="{656B0FA4-A7DA-4D70-9B17-633C6CD7B506}" presName="hierChild5" presStyleCnt="0"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{2E25BBEA-DA4E-4795-AB2E-4E623A9015ED}" type="pres">
+      <dgm:prSet presAssocID="{194D08C5-57EB-4155-B6F2-C4119AFD4E36}" presName="Name37" presStyleLbl="parChTrans1D2" presStyleIdx="2" presStyleCnt="5"/>
       <dgm:spPr/>
       <dgm:t>
         <a:bodyPr/>
@@ -1554,12 +1621,24 @@
         </a:p>
       </dgm:t>
     </dgm:pt>
-    <dgm:pt modelId="{8FCEA839-5421-4B25-A77C-B2B6C2C02558}" type="pres">
-      <dgm:prSet presAssocID="{50773849-F511-4835-AD5C-FC578FA128E4}" presName="hierChild4" presStyleCnt="0"/>
-      <dgm:spPr/>
-    </dgm:pt>
-    <dgm:pt modelId="{F4C3505A-509D-492B-A76D-03D866D48A9B}" type="pres">
-      <dgm:prSet presAssocID="{237A5FB3-0392-40DF-98C3-051D76C85975}" presName="Name37" presStyleLbl="parChTrans1D3" presStyleIdx="1" presStyleCnt="2"/>
+    <dgm:pt modelId="{75E405C0-9842-4565-8FB6-DDB1CAFFD11A}" type="pres">
+      <dgm:prSet presAssocID="{50773849-F511-4835-AD5C-FC578FA128E4}" presName="hierRoot2" presStyleCnt="0">
+        <dgm:presLayoutVars>
+          <dgm:hierBranch val="init"/>
+        </dgm:presLayoutVars>
+      </dgm:prSet>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{C7823C8D-F1A4-41A9-AAC6-90587AC45B04}" type="pres">
+      <dgm:prSet presAssocID="{50773849-F511-4835-AD5C-FC578FA128E4}" presName="rootComposite" presStyleCnt="0"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{747F2FED-B883-4887-A704-3213D63B59EB}" type="pres">
+      <dgm:prSet presAssocID="{50773849-F511-4835-AD5C-FC578FA128E4}" presName="rootText" presStyleLbl="node2" presStyleIdx="2" presStyleCnt="5">
+        <dgm:presLayoutVars>
+          <dgm:chPref val="3"/>
+        </dgm:presLayoutVars>
+      </dgm:prSet>
       <dgm:spPr/>
       <dgm:t>
         <a:bodyPr/>
@@ -1569,24 +1648,8 @@
         </a:p>
       </dgm:t>
     </dgm:pt>
-    <dgm:pt modelId="{6C87BF26-6704-4F24-B5DC-5F0E523ACA4C}" type="pres">
-      <dgm:prSet presAssocID="{B56F1F7B-9CAF-4E3C-8845-E5A0D88E4AC1}" presName="hierRoot2" presStyleCnt="0">
-        <dgm:presLayoutVars>
-          <dgm:hierBranch val="init"/>
-        </dgm:presLayoutVars>
-      </dgm:prSet>
-      <dgm:spPr/>
-    </dgm:pt>
-    <dgm:pt modelId="{AC6E90D5-E063-42D9-84FA-641E716E09D9}" type="pres">
-      <dgm:prSet presAssocID="{B56F1F7B-9CAF-4E3C-8845-E5A0D88E4AC1}" presName="rootComposite" presStyleCnt="0"/>
-      <dgm:spPr/>
-    </dgm:pt>
-    <dgm:pt modelId="{C9C249D0-F1D4-4554-A386-CAFA14270C36}" type="pres">
-      <dgm:prSet presAssocID="{B56F1F7B-9CAF-4E3C-8845-E5A0D88E4AC1}" presName="rootText" presStyleLbl="node3" presStyleIdx="1" presStyleCnt="2">
-        <dgm:presLayoutVars>
-          <dgm:chPref val="3"/>
-        </dgm:presLayoutVars>
-      </dgm:prSet>
+    <dgm:pt modelId="{D09303C9-BCC6-4DD2-8E33-C0F1AE38C831}" type="pres">
+      <dgm:prSet presAssocID="{50773849-F511-4835-AD5C-FC578FA128E4}" presName="rootConnector" presStyleLbl="node2" presStyleIdx="2" presStyleCnt="5"/>
       <dgm:spPr/>
       <dgm:t>
         <a:bodyPr/>
@@ -1596,8 +1659,12 @@
         </a:p>
       </dgm:t>
     </dgm:pt>
-    <dgm:pt modelId="{FFF9F715-5053-4613-89FA-1E0570F1C0C0}" type="pres">
-      <dgm:prSet presAssocID="{B56F1F7B-9CAF-4E3C-8845-E5A0D88E4AC1}" presName="rootConnector" presStyleLbl="node3" presStyleIdx="1" presStyleCnt="2"/>
+    <dgm:pt modelId="{8FCEA839-5421-4B25-A77C-B2B6C2C02558}" type="pres">
+      <dgm:prSet presAssocID="{50773849-F511-4835-AD5C-FC578FA128E4}" presName="hierChild4" presStyleCnt="0"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{F4C3505A-509D-492B-A76D-03D866D48A9B}" type="pres">
+      <dgm:prSet presAssocID="{237A5FB3-0392-40DF-98C3-051D76C85975}" presName="Name37" presStyleLbl="parChTrans1D3" presStyleIdx="1" presStyleCnt="2"/>
       <dgm:spPr/>
       <dgm:t>
         <a:bodyPr/>
@@ -1607,20 +1674,24 @@
         </a:p>
       </dgm:t>
     </dgm:pt>
-    <dgm:pt modelId="{803497FD-6163-4B62-AAA2-735D49D988DD}" type="pres">
-      <dgm:prSet presAssocID="{B56F1F7B-9CAF-4E3C-8845-E5A0D88E4AC1}" presName="hierChild4" presStyleCnt="0"/>
-      <dgm:spPr/>
-    </dgm:pt>
-    <dgm:pt modelId="{ACDCB1B2-5443-4038-80D4-CE277A515A25}" type="pres">
-      <dgm:prSet presAssocID="{B56F1F7B-9CAF-4E3C-8845-E5A0D88E4AC1}" presName="hierChild5" presStyleCnt="0"/>
-      <dgm:spPr/>
-    </dgm:pt>
-    <dgm:pt modelId="{B0CFFD3F-A927-4D27-97EA-5C803C05C1EC}" type="pres">
-      <dgm:prSet presAssocID="{50773849-F511-4835-AD5C-FC578FA128E4}" presName="hierChild5" presStyleCnt="0"/>
-      <dgm:spPr/>
-    </dgm:pt>
-    <dgm:pt modelId="{F2B1825C-8BC8-4111-A2C0-A0FBB338DE48}" type="pres">
-      <dgm:prSet presAssocID="{03BF1FA9-C075-4FA8-BD05-B802322534A6}" presName="Name37" presStyleLbl="parChTrans1D2" presStyleIdx="3" presStyleCnt="5"/>
+    <dgm:pt modelId="{6C87BF26-6704-4F24-B5DC-5F0E523ACA4C}" type="pres">
+      <dgm:prSet presAssocID="{B56F1F7B-9CAF-4E3C-8845-E5A0D88E4AC1}" presName="hierRoot2" presStyleCnt="0">
+        <dgm:presLayoutVars>
+          <dgm:hierBranch val="init"/>
+        </dgm:presLayoutVars>
+      </dgm:prSet>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{AC6E90D5-E063-42D9-84FA-641E716E09D9}" type="pres">
+      <dgm:prSet presAssocID="{B56F1F7B-9CAF-4E3C-8845-E5A0D88E4AC1}" presName="rootComposite" presStyleCnt="0"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{C9C249D0-F1D4-4554-A386-CAFA14270C36}" type="pres">
+      <dgm:prSet presAssocID="{B56F1F7B-9CAF-4E3C-8845-E5A0D88E4AC1}" presName="rootText" presStyleLbl="node3" presStyleIdx="1" presStyleCnt="2">
+        <dgm:presLayoutVars>
+          <dgm:chPref val="3"/>
+        </dgm:presLayoutVars>
+      </dgm:prSet>
       <dgm:spPr/>
       <dgm:t>
         <a:bodyPr/>
@@ -1630,24 +1701,8 @@
         </a:p>
       </dgm:t>
     </dgm:pt>
-    <dgm:pt modelId="{2F6718CB-1A8A-4650-AB72-E9A1BE671FFE}" type="pres">
-      <dgm:prSet presAssocID="{862D7E0D-F0D4-41D7-97A9-5B92A6FAF196}" presName="hierRoot2" presStyleCnt="0">
-        <dgm:presLayoutVars>
-          <dgm:hierBranch val="init"/>
-        </dgm:presLayoutVars>
-      </dgm:prSet>
-      <dgm:spPr/>
-    </dgm:pt>
-    <dgm:pt modelId="{1C50B8F7-B0D8-4AC7-9697-96D6DC8A6695}" type="pres">
-      <dgm:prSet presAssocID="{862D7E0D-F0D4-41D7-97A9-5B92A6FAF196}" presName="rootComposite" presStyleCnt="0"/>
-      <dgm:spPr/>
-    </dgm:pt>
-    <dgm:pt modelId="{B4A89E68-830E-49C7-8936-A684A6D977A9}" type="pres">
-      <dgm:prSet presAssocID="{862D7E0D-F0D4-41D7-97A9-5B92A6FAF196}" presName="rootText" presStyleLbl="node2" presStyleIdx="3" presStyleCnt="5">
-        <dgm:presLayoutVars>
-          <dgm:chPref val="3"/>
-        </dgm:presLayoutVars>
-      </dgm:prSet>
+    <dgm:pt modelId="{FFF9F715-5053-4613-89FA-1E0570F1C0C0}" type="pres">
+      <dgm:prSet presAssocID="{B56F1F7B-9CAF-4E3C-8845-E5A0D88E4AC1}" presName="rootConnector" presStyleLbl="node3" presStyleIdx="1" presStyleCnt="2"/>
       <dgm:spPr/>
       <dgm:t>
         <a:bodyPr/>
@@ -1657,8 +1712,20 @@
         </a:p>
       </dgm:t>
     </dgm:pt>
-    <dgm:pt modelId="{00785835-E3F4-4EF8-924A-607B1BE17BA3}" type="pres">
-      <dgm:prSet presAssocID="{862D7E0D-F0D4-41D7-97A9-5B92A6FAF196}" presName="rootConnector" presStyleLbl="node2" presStyleIdx="3" presStyleCnt="5"/>
+    <dgm:pt modelId="{803497FD-6163-4B62-AAA2-735D49D988DD}" type="pres">
+      <dgm:prSet presAssocID="{B56F1F7B-9CAF-4E3C-8845-E5A0D88E4AC1}" presName="hierChild4" presStyleCnt="0"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{ACDCB1B2-5443-4038-80D4-CE277A515A25}" type="pres">
+      <dgm:prSet presAssocID="{B56F1F7B-9CAF-4E3C-8845-E5A0D88E4AC1}" presName="hierChild5" presStyleCnt="0"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{B0CFFD3F-A927-4D27-97EA-5C803C05C1EC}" type="pres">
+      <dgm:prSet presAssocID="{50773849-F511-4835-AD5C-FC578FA128E4}" presName="hierChild5" presStyleCnt="0"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{F2B1825C-8BC8-4111-A2C0-A0FBB338DE48}" type="pres">
+      <dgm:prSet presAssocID="{03BF1FA9-C075-4FA8-BD05-B802322534A6}" presName="Name37" presStyleLbl="parChTrans1D2" presStyleIdx="3" presStyleCnt="5"/>
       <dgm:spPr/>
       <dgm:t>
         <a:bodyPr/>
@@ -1668,16 +1735,24 @@
         </a:p>
       </dgm:t>
     </dgm:pt>
-    <dgm:pt modelId="{7CDF85EA-A31C-46FE-AC6A-AA3C59759A2A}" type="pres">
-      <dgm:prSet presAssocID="{862D7E0D-F0D4-41D7-97A9-5B92A6FAF196}" presName="hierChild4" presStyleCnt="0"/>
-      <dgm:spPr/>
-    </dgm:pt>
-    <dgm:pt modelId="{2004B03C-06A2-4E4D-ABF4-8B17432697AE}" type="pres">
-      <dgm:prSet presAssocID="{862D7E0D-F0D4-41D7-97A9-5B92A6FAF196}" presName="hierChild5" presStyleCnt="0"/>
-      <dgm:spPr/>
-    </dgm:pt>
-    <dgm:pt modelId="{993DFE86-1DCA-48E6-AB6D-7101F7F884D6}" type="pres">
-      <dgm:prSet presAssocID="{89D5F964-69B4-4004-B7D0-88E04A580D4C}" presName="Name37" presStyleLbl="parChTrans1D2" presStyleIdx="4" presStyleCnt="5"/>
+    <dgm:pt modelId="{2F6718CB-1A8A-4650-AB72-E9A1BE671FFE}" type="pres">
+      <dgm:prSet presAssocID="{862D7E0D-F0D4-41D7-97A9-5B92A6FAF196}" presName="hierRoot2" presStyleCnt="0">
+        <dgm:presLayoutVars>
+          <dgm:hierBranch val="init"/>
+        </dgm:presLayoutVars>
+      </dgm:prSet>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{1C50B8F7-B0D8-4AC7-9697-96D6DC8A6695}" type="pres">
+      <dgm:prSet presAssocID="{862D7E0D-F0D4-41D7-97A9-5B92A6FAF196}" presName="rootComposite" presStyleCnt="0"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{B4A89E68-830E-49C7-8936-A684A6D977A9}" type="pres">
+      <dgm:prSet presAssocID="{862D7E0D-F0D4-41D7-97A9-5B92A6FAF196}" presName="rootText" presStyleLbl="node2" presStyleIdx="3" presStyleCnt="5">
+        <dgm:presLayoutVars>
+          <dgm:chPref val="3"/>
+        </dgm:presLayoutVars>
+      </dgm:prSet>
       <dgm:spPr/>
       <dgm:t>
         <a:bodyPr/>
@@ -1687,24 +1762,8 @@
         </a:p>
       </dgm:t>
     </dgm:pt>
-    <dgm:pt modelId="{C8B37CB4-59A5-4030-AA67-752675154247}" type="pres">
-      <dgm:prSet presAssocID="{AE8947B9-4DD1-4CBA-876B-A4D5D8B01A87}" presName="hierRoot2" presStyleCnt="0">
-        <dgm:presLayoutVars>
-          <dgm:hierBranch val="init"/>
-        </dgm:presLayoutVars>
-      </dgm:prSet>
-      <dgm:spPr/>
-    </dgm:pt>
-    <dgm:pt modelId="{17CD3FE5-42A0-4E0F-9D5C-426B3CBDC113}" type="pres">
-      <dgm:prSet presAssocID="{AE8947B9-4DD1-4CBA-876B-A4D5D8B01A87}" presName="rootComposite" presStyleCnt="0"/>
-      <dgm:spPr/>
-    </dgm:pt>
-    <dgm:pt modelId="{77618643-8909-4B96-B865-0D76F6C6AC5C}" type="pres">
-      <dgm:prSet presAssocID="{AE8947B9-4DD1-4CBA-876B-A4D5D8B01A87}" presName="rootText" presStyleLbl="node2" presStyleIdx="4" presStyleCnt="5">
-        <dgm:presLayoutVars>
-          <dgm:chPref val="3"/>
-        </dgm:presLayoutVars>
-      </dgm:prSet>
+    <dgm:pt modelId="{00785835-E3F4-4EF8-924A-607B1BE17BA3}" type="pres">
+      <dgm:prSet presAssocID="{862D7E0D-F0D4-41D7-97A9-5B92A6FAF196}" presName="rootConnector" presStyleLbl="node2" presStyleIdx="3" presStyleCnt="5"/>
       <dgm:spPr/>
       <dgm:t>
         <a:bodyPr/>
@@ -1714,8 +1773,16 @@
         </a:p>
       </dgm:t>
     </dgm:pt>
-    <dgm:pt modelId="{82DF419B-8EE6-4CB7-BAB1-86FC9D1E9AC1}" type="pres">
-      <dgm:prSet presAssocID="{AE8947B9-4DD1-4CBA-876B-A4D5D8B01A87}" presName="rootConnector" presStyleLbl="node2" presStyleIdx="4" presStyleCnt="5"/>
+    <dgm:pt modelId="{7CDF85EA-A31C-46FE-AC6A-AA3C59759A2A}" type="pres">
+      <dgm:prSet presAssocID="{862D7E0D-F0D4-41D7-97A9-5B92A6FAF196}" presName="hierChild4" presStyleCnt="0"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{2004B03C-06A2-4E4D-ABF4-8B17432697AE}" type="pres">
+      <dgm:prSet presAssocID="{862D7E0D-F0D4-41D7-97A9-5B92A6FAF196}" presName="hierChild5" presStyleCnt="0"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{993DFE86-1DCA-48E6-AB6D-7101F7F884D6}" type="pres">
+      <dgm:prSet presAssocID="{89D5F964-69B4-4004-B7D0-88E04A580D4C}" presName="Name37" presStyleLbl="parChTrans1D2" presStyleIdx="4" presStyleCnt="5"/>
       <dgm:spPr/>
       <dgm:t>
         <a:bodyPr/>
@@ -1725,6 +1792,44 @@
         </a:p>
       </dgm:t>
     </dgm:pt>
+    <dgm:pt modelId="{C8B37CB4-59A5-4030-AA67-752675154247}" type="pres">
+      <dgm:prSet presAssocID="{AE8947B9-4DD1-4CBA-876B-A4D5D8B01A87}" presName="hierRoot2" presStyleCnt="0">
+        <dgm:presLayoutVars>
+          <dgm:hierBranch val="init"/>
+        </dgm:presLayoutVars>
+      </dgm:prSet>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{17CD3FE5-42A0-4E0F-9D5C-426B3CBDC113}" type="pres">
+      <dgm:prSet presAssocID="{AE8947B9-4DD1-4CBA-876B-A4D5D8B01A87}" presName="rootComposite" presStyleCnt="0"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{77618643-8909-4B96-B865-0D76F6C6AC5C}" type="pres">
+      <dgm:prSet presAssocID="{AE8947B9-4DD1-4CBA-876B-A4D5D8B01A87}" presName="rootText" presStyleLbl="node2" presStyleIdx="4" presStyleCnt="5">
+        <dgm:presLayoutVars>
+          <dgm:chPref val="3"/>
+        </dgm:presLayoutVars>
+      </dgm:prSet>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="pl-PL"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{82DF419B-8EE6-4CB7-BAB1-86FC9D1E9AC1}" type="pres">
+      <dgm:prSet presAssocID="{AE8947B9-4DD1-4CBA-876B-A4D5D8B01A87}" presName="rootConnector" presStyleLbl="node2" presStyleIdx="4" presStyleCnt="5"/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="pl-PL"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
     <dgm:pt modelId="{AB06BFB8-3302-441D-AE77-152478D7B0A2}" type="pres">
       <dgm:prSet presAssocID="{AE8947B9-4DD1-4CBA-876B-A4D5D8B01A87}" presName="hierChild4" presStyleCnt="0"/>
       <dgm:spPr/>
@@ -1740,37 +1845,41 @@
   </dgm:ptLst>
   <dgm:cxnLst>
     <dgm:cxn modelId="{8BE19EC5-B58E-4BB9-94F6-ED249D783BE0}" type="presOf" srcId="{F869AEC1-1E83-4EF1-A608-2ED7273BDA79}" destId="{E326ADC5-C67D-47B5-8B70-410250FC4F45}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{0571FFFF-892A-4489-BC21-50013D5FAFB8}" type="presOf" srcId="{656B0FA4-A7DA-4D70-9B17-633C6CD7B506}" destId="{BE5A54D6-F6AF-424F-9423-F66B0C5B6243}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{02C98010-6CFF-47EB-983D-ABB138E78C3F}" type="presOf" srcId="{C1626232-3005-446D-A578-0D8DD393590B}" destId="{D696FE8C-BF81-4065-B3CB-3252DA3B830C}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{D22151FF-90F3-4064-AF05-2D331A6447FF}" type="presOf" srcId="{0D581458-B5EE-4A7F-90FD-3F9112FA4B78}" destId="{2928310D-2CA9-4834-90E6-7BDF49776789}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{EBAD0603-3220-4C69-9DAB-8C0B4DD3570D}" type="presOf" srcId="{31984FD3-2923-4172-BF0B-1AD9B9A01FD5}" destId="{6FC1C387-5713-4261-B66C-02A4F0A263E3}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{CD61DB0A-B629-49DD-B878-4C06AA3A3AE8}" srcId="{90625BEE-1CE8-4E94-BD93-26C691FBA331}" destId="{F869AEC1-1E83-4EF1-A608-2ED7273BDA79}" srcOrd="0" destOrd="0" parTransId="{C1626232-3005-446D-A578-0D8DD393590B}" sibTransId="{6452D633-FE9F-435E-9089-7302FF61B0B4}"/>
+    <dgm:cxn modelId="{AD493D86-C543-4015-BE87-29F68962786B}" type="presOf" srcId="{862D7E0D-F0D4-41D7-97A9-5B92A6FAF196}" destId="{B4A89E68-830E-49C7-8936-A684A6D977A9}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{BBBBFC24-5922-4864-9A93-7D550876B03D}" srcId="{90625BEE-1CE8-4E94-BD93-26C691FBA331}" destId="{656B0FA4-A7DA-4D70-9B17-633C6CD7B506}" srcOrd="1" destOrd="0" parTransId="{23DA1795-4ACE-4459-B5FA-3766EB5DF9C5}" sibTransId="{8D6D3067-77F2-44F8-AE5E-4D8FF3F2F5B2}"/>
+    <dgm:cxn modelId="{5B2F66D6-2E7D-4412-81A9-A3C99C3D835D}" type="presOf" srcId="{4FB2B5CC-B5E8-4444-9946-1293B3748920}" destId="{CCD8050B-E3A1-4D78-A2EC-AF861030206E}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{FC46046D-CE9D-4FB8-9DC6-2EA1C1776976}" type="presOf" srcId="{656B0FA4-A7DA-4D70-9B17-633C6CD7B506}" destId="{638ED046-8A50-4647-BF8C-DC993BB3E9B8}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{A0DB7B1F-CF71-4EF2-8DF4-231F649ACACD}" type="presOf" srcId="{50773849-F511-4835-AD5C-FC578FA128E4}" destId="{747F2FED-B883-4887-A704-3213D63B59EB}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
     <dgm:cxn modelId="{DD52EC3C-F2CD-484A-9560-578DFDD6F601}" type="presOf" srcId="{B56F1F7B-9CAF-4E3C-8845-E5A0D88E4AC1}" destId="{C9C249D0-F1D4-4554-A386-CAFA14270C36}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{71E0349D-088D-4E65-A8C6-D6879D89E856}" type="presOf" srcId="{03BF1FA9-C075-4FA8-BD05-B802322534A6}" destId="{F2B1825C-8BC8-4111-A2C0-A0FBB338DE48}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{07549231-1028-4839-90EE-ED2D4CFA9008}" srcId="{90625BEE-1CE8-4E94-BD93-26C691FBA331}" destId="{AE8947B9-4DD1-4CBA-876B-A4D5D8B01A87}" srcOrd="4" destOrd="0" parTransId="{89D5F964-69B4-4004-B7D0-88E04A580D4C}" sibTransId="{74E6B8B5-04F1-47B0-B758-FDE2DD2D1E84}"/>
+    <dgm:cxn modelId="{21BE257A-D0D0-4391-BE49-CB8903F75F88}" srcId="{90625BEE-1CE8-4E94-BD93-26C691FBA331}" destId="{50773849-F511-4835-AD5C-FC578FA128E4}" srcOrd="2" destOrd="0" parTransId="{194D08C5-57EB-4155-B6F2-C4119AFD4E36}" sibTransId="{153384F9-AE57-4070-8EA4-71D24C7CF196}"/>
+    <dgm:cxn modelId="{63E4C16F-DAFF-4115-824D-4E5062F2889B}" type="presOf" srcId="{90625BEE-1CE8-4E94-BD93-26C691FBA331}" destId="{0508117B-3BAB-41D1-94DF-0CF04275C7FA}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{58D39FB8-3B72-436D-B378-75D5CFD0C8F7}" srcId="{90625BEE-1CE8-4E94-BD93-26C691FBA331}" destId="{862D7E0D-F0D4-41D7-97A9-5B92A6FAF196}" srcOrd="3" destOrd="0" parTransId="{03BF1FA9-C075-4FA8-BD05-B802322534A6}" sibTransId="{C266CAE2-4D1C-4F15-A627-AE1D114514FC}"/>
+    <dgm:cxn modelId="{9B39BB91-BCA2-4F88-A888-A93460ACAC0D}" srcId="{656B0FA4-A7DA-4D70-9B17-633C6CD7B506}" destId="{A6185CF1-A6C9-4057-B034-F738C98E78D8}" srcOrd="0" destOrd="0" parTransId="{4FB2B5CC-B5E8-4444-9946-1293B3748920}" sibTransId="{E6879C87-8E8C-49ED-9950-ECD513F23E89}"/>
+    <dgm:cxn modelId="{B0173BF3-1663-4869-9510-FF3E6ECDB80B}" type="presOf" srcId="{90625BEE-1CE8-4E94-BD93-26C691FBA331}" destId="{96CAB6C0-43D1-4509-B5E4-801A2235C3C0}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{1901550F-B5B2-4B92-9703-D60185DDB73A}" type="presOf" srcId="{4E1CD3DD-F8B4-4A0F-97E8-1A1E5C772D18}" destId="{ACC15529-EE74-465D-8E76-84913ECA718C}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{DCBE64CE-AD06-4484-A607-7AE8805AA703}" type="presOf" srcId="{50773849-F511-4835-AD5C-FC578FA128E4}" destId="{D09303C9-BCC6-4DD2-8E33-C0F1AE38C831}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
     <dgm:cxn modelId="{325DAB41-614B-4868-B08A-5032FB3CA0F3}" srcId="{50773849-F511-4835-AD5C-FC578FA128E4}" destId="{B56F1F7B-9CAF-4E3C-8845-E5A0D88E4AC1}" srcOrd="0" destOrd="0" parTransId="{237A5FB3-0392-40DF-98C3-051D76C85975}" sibTransId="{D9AC3E19-03F8-4B24-9C05-1F58DDABFDD4}"/>
     <dgm:cxn modelId="{A02A8C92-53D2-400A-8E31-C1D36C74C310}" type="presOf" srcId="{A6185CF1-A6C9-4057-B034-F738C98E78D8}" destId="{488D30EC-5368-42BE-91A5-E867C0D7A783}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{71E0349D-088D-4E65-A8C6-D6879D89E856}" type="presOf" srcId="{03BF1FA9-C075-4FA8-BD05-B802322534A6}" destId="{F2B1825C-8BC8-4111-A2C0-A0FBB338DE48}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
     <dgm:cxn modelId="{B64F773A-90DB-49B8-A18F-5E4035FFF432}" srcId="{0D581458-B5EE-4A7F-90FD-3F9112FA4B78}" destId="{90625BEE-1CE8-4E94-BD93-26C691FBA331}" srcOrd="0" destOrd="0" parTransId="{0F3A10AD-3B79-4301-B641-B9A7875FF524}" sibTransId="{9544EE45-59CE-4B8F-A53E-FCC70B170D25}"/>
-    <dgm:cxn modelId="{02C98010-6CFF-47EB-983D-ABB138E78C3F}" type="presOf" srcId="{C1626232-3005-446D-A578-0D8DD393590B}" destId="{D696FE8C-BF81-4065-B3CB-3252DA3B830C}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{63E4C16F-DAFF-4115-824D-4E5062F2889B}" type="presOf" srcId="{90625BEE-1CE8-4E94-BD93-26C691FBA331}" destId="{0508117B-3BAB-41D1-94DF-0CF04275C7FA}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{58D39FB8-3B72-436D-B378-75D5CFD0C8F7}" srcId="{90625BEE-1CE8-4E94-BD93-26C691FBA331}" destId="{862D7E0D-F0D4-41D7-97A9-5B92A6FAF196}" srcOrd="3" destOrd="0" parTransId="{03BF1FA9-C075-4FA8-BD05-B802322534A6}" sibTransId="{C266CAE2-4D1C-4F15-A627-AE1D114514FC}"/>
-    <dgm:cxn modelId="{B0173BF3-1663-4869-9510-FF3E6ECDB80B}" type="presOf" srcId="{90625BEE-1CE8-4E94-BD93-26C691FBA331}" destId="{96CAB6C0-43D1-4509-B5E4-801A2235C3C0}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{80690E98-44DE-474F-96AD-37737EBE6006}" type="presOf" srcId="{862D7E0D-F0D4-41D7-97A9-5B92A6FAF196}" destId="{00785835-E3F4-4EF8-924A-607B1BE17BA3}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{E32E1CDD-73E3-42B3-A0EA-B3D9D6F682C3}" type="presOf" srcId="{B56F1F7B-9CAF-4E3C-8845-E5A0D88E4AC1}" destId="{FFF9F715-5053-4613-89FA-1E0570F1C0C0}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{F89E3577-23BC-4092-A78D-6926C637E5D1}" type="presOf" srcId="{F869AEC1-1E83-4EF1-A608-2ED7273BDA79}" destId="{C57A6536-4127-4AA1-8522-04474917B5F5}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{1974D637-A2B6-4A9D-835D-F75A876943E7}" type="presOf" srcId="{23DA1795-4ACE-4459-B5FA-3766EB5DF9C5}" destId="{8B733281-3DE3-4C42-A883-193A9A249CD6}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{BF396FEA-265D-4E32-A5F2-137B0774A15F}" type="presOf" srcId="{AE8947B9-4DD1-4CBA-876B-A4D5D8B01A87}" destId="{77618643-8909-4B96-B865-0D76F6C6AC5C}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
     <dgm:cxn modelId="{C56E1D74-B152-4B9F-8564-CBCE6D400DF6}" type="presOf" srcId="{A6185CF1-A6C9-4057-B034-F738C98E78D8}" destId="{32A9C23E-AD8C-4291-91FD-D6B43BE6B459}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{0F9AB5E7-E337-4889-AB7C-6F392B74B41B}" type="presOf" srcId="{237A5FB3-0392-40DF-98C3-051D76C85975}" destId="{F4C3505A-509D-492B-A76D-03D866D48A9B}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{1FD79E27-935D-44F1-A586-B49C57823F68}" type="presOf" srcId="{89D5F964-69B4-4004-B7D0-88E04A580D4C}" destId="{993DFE86-1DCA-48E6-AB6D-7101F7F884D6}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{2CA843AA-07B2-4DA0-A5CB-01A56720AC23}" type="presOf" srcId="{31984FD3-2923-4172-BF0B-1AD9B9A01FD5}" destId="{71963852-35F0-42CE-850C-B12317072D70}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{0571FFFF-892A-4489-BC21-50013D5FAFB8}" type="presOf" srcId="{656B0FA4-A7DA-4D70-9B17-633C6CD7B506}" destId="{BE5A54D6-F6AF-424F-9423-F66B0C5B6243}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{CC4146FF-ADDE-46CB-BD84-61F7CA13E7EC}" srcId="{A6185CF1-A6C9-4057-B034-F738C98E78D8}" destId="{31984FD3-2923-4172-BF0B-1AD9B9A01FD5}" srcOrd="0" destOrd="0" parTransId="{4E1CD3DD-F8B4-4A0F-97E8-1A1E5C772D18}" sibTransId="{5F56B929-C765-4B7E-81DE-6F334B61057E}"/>
+    <dgm:cxn modelId="{5C199323-C776-407F-B4A7-96CE1F728BFC}" type="presOf" srcId="{AE8947B9-4DD1-4CBA-876B-A4D5D8B01A87}" destId="{82DF419B-8EE6-4CB7-BAB1-86FC9D1E9AC1}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
     <dgm:cxn modelId="{1DD651EF-393A-4ECA-BDA5-58D00B75F246}" type="presOf" srcId="{194D08C5-57EB-4155-B6F2-C4119AFD4E36}" destId="{2E25BBEA-DA4E-4795-AB2E-4E623A9015ED}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{BF396FEA-265D-4E32-A5F2-137B0774A15F}" type="presOf" srcId="{AE8947B9-4DD1-4CBA-876B-A4D5D8B01A87}" destId="{77618643-8909-4B96-B865-0D76F6C6AC5C}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{D22151FF-90F3-4064-AF05-2D331A6447FF}" type="presOf" srcId="{0D581458-B5EE-4A7F-90FD-3F9112FA4B78}" destId="{2928310D-2CA9-4834-90E6-7BDF49776789}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{AD493D86-C543-4015-BE87-29F68962786B}" type="presOf" srcId="{862D7E0D-F0D4-41D7-97A9-5B92A6FAF196}" destId="{B4A89E68-830E-49C7-8936-A684A6D977A9}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{F89E3577-23BC-4092-A78D-6926C637E5D1}" type="presOf" srcId="{F869AEC1-1E83-4EF1-A608-2ED7273BDA79}" destId="{C57A6536-4127-4AA1-8522-04474917B5F5}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{07549231-1028-4839-90EE-ED2D4CFA9008}" srcId="{90625BEE-1CE8-4E94-BD93-26C691FBA331}" destId="{AE8947B9-4DD1-4CBA-876B-A4D5D8B01A87}" srcOrd="4" destOrd="0" parTransId="{89D5F964-69B4-4004-B7D0-88E04A580D4C}" sibTransId="{74E6B8B5-04F1-47B0-B758-FDE2DD2D1E84}"/>
-    <dgm:cxn modelId="{A0DB7B1F-CF71-4EF2-8DF4-231F649ACACD}" type="presOf" srcId="{50773849-F511-4835-AD5C-FC578FA128E4}" destId="{747F2FED-B883-4887-A704-3213D63B59EB}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{80690E98-44DE-474F-96AD-37737EBE6006}" type="presOf" srcId="{862D7E0D-F0D4-41D7-97A9-5B92A6FAF196}" destId="{00785835-E3F4-4EF8-924A-607B1BE17BA3}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{BBBBFC24-5922-4864-9A93-7D550876B03D}" srcId="{90625BEE-1CE8-4E94-BD93-26C691FBA331}" destId="{656B0FA4-A7DA-4D70-9B17-633C6CD7B506}" srcOrd="1" destOrd="0" parTransId="{23DA1795-4ACE-4459-B5FA-3766EB5DF9C5}" sibTransId="{8D6D3067-77F2-44F8-AE5E-4D8FF3F2F5B2}"/>
-    <dgm:cxn modelId="{1FD79E27-935D-44F1-A586-B49C57823F68}" type="presOf" srcId="{89D5F964-69B4-4004-B7D0-88E04A580D4C}" destId="{993DFE86-1DCA-48E6-AB6D-7101F7F884D6}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{E32E1CDD-73E3-42B3-A0EA-B3D9D6F682C3}" type="presOf" srcId="{B56F1F7B-9CAF-4E3C-8845-E5A0D88E4AC1}" destId="{FFF9F715-5053-4613-89FA-1E0570F1C0C0}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{0F9AB5E7-E337-4889-AB7C-6F392B74B41B}" type="presOf" srcId="{237A5FB3-0392-40DF-98C3-051D76C85975}" destId="{F4C3505A-509D-492B-A76D-03D866D48A9B}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{FC46046D-CE9D-4FB8-9DC6-2EA1C1776976}" type="presOf" srcId="{656B0FA4-A7DA-4D70-9B17-633C6CD7B506}" destId="{638ED046-8A50-4647-BF8C-DC993BB3E9B8}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{CD61DB0A-B629-49DD-B878-4C06AA3A3AE8}" srcId="{90625BEE-1CE8-4E94-BD93-26C691FBA331}" destId="{F869AEC1-1E83-4EF1-A608-2ED7273BDA79}" srcOrd="0" destOrd="0" parTransId="{C1626232-3005-446D-A578-0D8DD393590B}" sibTransId="{6452D633-FE9F-435E-9089-7302FF61B0B4}"/>
-    <dgm:cxn modelId="{5C199323-C776-407F-B4A7-96CE1F728BFC}" type="presOf" srcId="{AE8947B9-4DD1-4CBA-876B-A4D5D8B01A87}" destId="{82DF419B-8EE6-4CB7-BAB1-86FC9D1E9AC1}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{9B39BB91-BCA2-4F88-A888-A93460ACAC0D}" srcId="{656B0FA4-A7DA-4D70-9B17-633C6CD7B506}" destId="{A6185CF1-A6C9-4057-B034-F738C98E78D8}" srcOrd="0" destOrd="0" parTransId="{4FB2B5CC-B5E8-4444-9946-1293B3748920}" sibTransId="{E6879C87-8E8C-49ED-9950-ECD513F23E89}"/>
-    <dgm:cxn modelId="{1974D637-A2B6-4A9D-835D-F75A876943E7}" type="presOf" srcId="{23DA1795-4ACE-4459-B5FA-3766EB5DF9C5}" destId="{8B733281-3DE3-4C42-A883-193A9A249CD6}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{21BE257A-D0D0-4391-BE49-CB8903F75F88}" srcId="{90625BEE-1CE8-4E94-BD93-26C691FBA331}" destId="{50773849-F511-4835-AD5C-FC578FA128E4}" srcOrd="2" destOrd="0" parTransId="{194D08C5-57EB-4155-B6F2-C4119AFD4E36}" sibTransId="{153384F9-AE57-4070-8EA4-71D24C7CF196}"/>
-    <dgm:cxn modelId="{5B2F66D6-2E7D-4412-81A9-A3C99C3D835D}" type="presOf" srcId="{4FB2B5CC-B5E8-4444-9946-1293B3748920}" destId="{CCD8050B-E3A1-4D78-A2EC-AF861030206E}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{DCBE64CE-AD06-4484-A607-7AE8805AA703}" type="presOf" srcId="{50773849-F511-4835-AD5C-FC578FA128E4}" destId="{D09303C9-BCC6-4DD2-8E33-C0F1AE38C831}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
     <dgm:cxn modelId="{546EAD4A-7D6C-4C9E-8694-592BA2714166}" type="presParOf" srcId="{2928310D-2CA9-4834-90E6-7BDF49776789}" destId="{B2DCFB66-D7FB-48ED-BCA0-9F369E1668C2}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
     <dgm:cxn modelId="{1B4AF8C2-0FBB-4AB5-AB2E-2CD5CDD6F28E}" type="presParOf" srcId="{B2DCFB66-D7FB-48ED-BCA0-9F369E1668C2}" destId="{EAC19A42-ACBD-4DEC-9558-1A920DBAF4EA}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
     <dgm:cxn modelId="{A910809D-AC77-42E6-B902-1CEB623229D4}" type="presParOf" srcId="{EAC19A42-ACBD-4DEC-9558-1A920DBAF4EA}" destId="{0508117B-3BAB-41D1-94DF-0CF04275C7FA}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
@@ -1795,6 +1904,13 @@
     <dgm:cxn modelId="{5138C4B3-E608-4D7B-B84A-2D1BA674077C}" type="presParOf" srcId="{11538DA3-0FFC-4D24-8D5B-B452CCE01884}" destId="{488D30EC-5368-42BE-91A5-E867C0D7A783}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
     <dgm:cxn modelId="{87605DE3-E009-4696-9C25-DCF7365ABA3F}" type="presParOf" srcId="{11538DA3-0FFC-4D24-8D5B-B452CCE01884}" destId="{32A9C23E-AD8C-4291-91FD-D6B43BE6B459}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
     <dgm:cxn modelId="{097408C7-54B1-4E98-8155-F785794A5162}" type="presParOf" srcId="{91320BF6-D109-4A45-B16D-C705B74FD78D}" destId="{E16D2A24-4E46-4D94-9851-37881F0781E6}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{F3D4DBA8-0E6E-438D-992E-6855F91E7DCD}" type="presParOf" srcId="{E16D2A24-4E46-4D94-9851-37881F0781E6}" destId="{ACC15529-EE74-465D-8E76-84913ECA718C}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{38F8A3F7-3116-4D84-AE59-264083754C8C}" type="presParOf" srcId="{E16D2A24-4E46-4D94-9851-37881F0781E6}" destId="{EB97A818-6508-4738-A451-20FFF43ED8D6}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{03622FCD-E49E-4C09-A1F7-4FE4E11547DA}" type="presParOf" srcId="{EB97A818-6508-4738-A451-20FFF43ED8D6}" destId="{F4F92C47-4DB4-4F3D-AF9B-3AA6C3E64951}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{6A7B3676-AC9E-42C1-9EE2-BB6CD92A92B4}" type="presParOf" srcId="{F4F92C47-4DB4-4F3D-AF9B-3AA6C3E64951}" destId="{71963852-35F0-42CE-850C-B12317072D70}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{E498235A-E38C-488B-8EE8-F26A13285FDA}" type="presParOf" srcId="{F4F92C47-4DB4-4F3D-AF9B-3AA6C3E64951}" destId="{6FC1C387-5713-4261-B66C-02A4F0A263E3}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{822E9E8D-E6D7-456A-99B1-67BCC4D8D21C}" type="presParOf" srcId="{EB97A818-6508-4738-A451-20FFF43ED8D6}" destId="{FAEFEE1A-3D8E-455A-B487-F61EB5EA8FE0}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{CE88175F-E2D1-47B7-A2F4-41AD4942E69C}" type="presParOf" srcId="{EB97A818-6508-4738-A451-20FFF43ED8D6}" destId="{279CE8DD-7BE7-47A8-872B-FF55B77EB153}" srcOrd="2" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
     <dgm:cxn modelId="{5DB477B0-9581-4BE0-9276-70E45BF5545A}" type="presParOf" srcId="{91320BF6-D109-4A45-B16D-C705B74FD78D}" destId="{E7F26332-31D7-4D14-887D-38AC3F6B542D}" srcOrd="2" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
     <dgm:cxn modelId="{682AEB33-C171-4E83-B54B-1922E30E704B}" type="presParOf" srcId="{75AFD5F6-2F24-454A-84AD-345A8872FBE7}" destId="{5196F5DF-44C1-47A9-A6ED-F4D25A01B422}" srcOrd="2" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
     <dgm:cxn modelId="{84D62002-2B35-4136-A1BD-0C0985E7B886}" type="presParOf" srcId="{E11E15A6-B9E1-4464-ACAB-B8B240A9A4D9}" destId="{2E25BBEA-DA4E-4795-AB2E-4E623A9015ED}" srcOrd="4" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
@@ -1852,7 +1968,7 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="2605087" y="2256679"/>
+          <a:off x="2605087" y="2321019"/>
           <a:ext cx="2158641" cy="187320"/>
         </a:xfrm>
         <a:custGeom>
@@ -1913,7 +2029,7 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="2605087" y="2256679"/>
+          <a:off x="2605087" y="2321019"/>
           <a:ext cx="1079320" cy="187320"/>
         </a:xfrm>
         <a:custGeom>
@@ -1974,7 +2090,7 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="2248287" y="2890000"/>
+          <a:off x="2248287" y="2954339"/>
           <a:ext cx="133800" cy="410320"/>
         </a:xfrm>
         <a:custGeom>
@@ -2032,7 +2148,7 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="2559367" y="2256679"/>
+          <a:off x="2559367" y="2321019"/>
           <a:ext cx="91440" cy="187320"/>
         </a:xfrm>
         <a:custGeom>
@@ -2080,14 +2196,14 @@
         <a:fontRef idx="minor"/>
       </dsp:style>
     </dsp:sp>
-    <dsp:sp modelId="{CCD8050B-E3A1-4D78-A2EC-AF861030206E}">
+    <dsp:sp modelId="{ACC15529-EE74-465D-8E76-84913ECA718C}">
       <dsp:nvSpPr>
         <dsp:cNvPr id="0" name=""/>
         <dsp:cNvSpPr/>
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="1168966" y="2890000"/>
+          <a:off x="1168966" y="3587660"/>
           <a:ext cx="133800" cy="410320"/>
         </a:xfrm>
         <a:custGeom>
@@ -2138,6 +2254,61 @@
         <a:fontRef idx="minor"/>
       </dsp:style>
     </dsp:sp>
+    <dsp:sp modelId="{CCD8050B-E3A1-4D78-A2EC-AF861030206E}">
+      <dsp:nvSpPr>
+        <dsp:cNvPr id="0" name=""/>
+        <dsp:cNvSpPr/>
+      </dsp:nvSpPr>
+      <dsp:spPr>
+        <a:xfrm>
+          <a:off x="1480046" y="2954339"/>
+          <a:ext cx="91440" cy="187320"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst>
+            <a:path>
+              <a:moveTo>
+                <a:pt x="45720" y="0"/>
+              </a:moveTo>
+              <a:lnTo>
+                <a:pt x="45720" y="187320"/>
+              </a:lnTo>
+            </a:path>
+          </a:pathLst>
+        </a:custGeom>
+        <a:noFill/>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="accent1">
+              <a:shade val="80000"/>
+              <a:hueOff val="0"/>
+              <a:satOff val="0"/>
+              <a:lumOff val="0"/>
+              <a:alphaOff val="0"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:effectLst/>
+      </dsp:spPr>
+      <dsp:style>
+        <a:lnRef idx="2">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor"/>
+      </dsp:style>
+    </dsp:sp>
     <dsp:sp modelId="{8B733281-3DE3-4C42-A883-193A9A249CD6}">
       <dsp:nvSpPr>
         <dsp:cNvPr id="0" name=""/>
@@ -2145,7 +2316,7 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="1525766" y="2256679"/>
+          <a:off x="1525766" y="2321019"/>
           <a:ext cx="1079320" cy="187320"/>
         </a:xfrm>
         <a:custGeom>
@@ -2206,7 +2377,7 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="446445" y="2256679"/>
+          <a:off x="446445" y="2321019"/>
           <a:ext cx="2158641" cy="187320"/>
         </a:xfrm>
         <a:custGeom>
@@ -2267,7 +2438,7 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="2159087" y="1810679"/>
+          <a:off x="2159087" y="1875018"/>
           <a:ext cx="892000" cy="446000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2332,7 +2503,7 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="2159087" y="1810679"/>
+        <a:off x="2159087" y="1875018"/>
         <a:ext cx="892000" cy="446000"/>
       </dsp:txXfrm>
     </dsp:sp>
@@ -2343,7 +2514,7 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="445" y="2443999"/>
+          <a:off x="445" y="2508339"/>
           <a:ext cx="892000" cy="446000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2408,7 +2579,7 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="445" y="2443999"/>
+        <a:off x="445" y="2508339"/>
         <a:ext cx="892000" cy="446000"/>
       </dsp:txXfrm>
     </dsp:sp>
@@ -2419,7 +2590,7 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="1079766" y="2443999"/>
+          <a:off x="1079766" y="2508339"/>
           <a:ext cx="892000" cy="446000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2484,7 +2655,7 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="1079766" y="2443999"/>
+        <a:off x="1079766" y="2508339"/>
         <a:ext cx="892000" cy="446000"/>
       </dsp:txXfrm>
     </dsp:sp>
@@ -2495,7 +2666,7 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="1302766" y="3077320"/>
+          <a:off x="1079766" y="3141660"/>
           <a:ext cx="892000" cy="446000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2560,7 +2731,83 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="1302766" y="3077320"/>
+        <a:off x="1079766" y="3141660"/>
+        <a:ext cx="892000" cy="446000"/>
+      </dsp:txXfrm>
+    </dsp:sp>
+    <dsp:sp modelId="{71963852-35F0-42CE-850C-B12317072D70}">
+      <dsp:nvSpPr>
+        <dsp:cNvPr id="0" name=""/>
+        <dsp:cNvSpPr/>
+      </dsp:nvSpPr>
+      <dsp:spPr>
+        <a:xfrm>
+          <a:off x="1302766" y="3774980"/>
+          <a:ext cx="892000" cy="446000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent1">
+            <a:hueOff val="0"/>
+            <a:satOff val="0"/>
+            <a:lumOff val="0"/>
+            <a:alphaOff val="0"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:hueOff val="0"/>
+              <a:satOff val="0"/>
+              <a:lumOff val="0"/>
+              <a:alphaOff val="0"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:effectLst/>
+      </dsp:spPr>
+      <dsp:style>
+        <a:lnRef idx="2">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </dsp:style>
+      <dsp:txBody>
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="5715" tIns="5715" rIns="5715" bIns="5715" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr lvl="0" algn="ctr" defTabSz="400050">
+            <a:lnSpc>
+              <a:spcPct val="90000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPct val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPct val="35000"/>
+            </a:spcAft>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="pl-PL" sz="900" kern="1200"/>
+            <a:t>img_src</a:t>
+          </a:r>
+        </a:p>
+      </dsp:txBody>
+      <dsp:txXfrm>
+        <a:off x="1302766" y="3774980"/>
         <a:ext cx="892000" cy="446000"/>
       </dsp:txXfrm>
     </dsp:sp>
@@ -2571,7 +2818,7 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="2159087" y="2443999"/>
+          <a:off x="2159087" y="2508339"/>
           <a:ext cx="892000" cy="446000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2636,7 +2883,7 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="2159087" y="2443999"/>
+        <a:off x="2159087" y="2508339"/>
         <a:ext cx="892000" cy="446000"/>
       </dsp:txXfrm>
     </dsp:sp>
@@ -2647,7 +2894,7 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="2382087" y="3077320"/>
+          <a:off x="2382087" y="3141660"/>
           <a:ext cx="892000" cy="446000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2712,7 +2959,7 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="2382087" y="3077320"/>
+        <a:off x="2382087" y="3141660"/>
         <a:ext cx="892000" cy="446000"/>
       </dsp:txXfrm>
     </dsp:sp>
@@ -2723,7 +2970,7 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="3238408" y="2443999"/>
+          <a:off x="3238408" y="2508339"/>
           <a:ext cx="892000" cy="446000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2788,7 +3035,7 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="3238408" y="2443999"/>
+        <a:off x="3238408" y="2508339"/>
         <a:ext cx="892000" cy="446000"/>
       </dsp:txXfrm>
     </dsp:sp>
@@ -2799,7 +3046,7 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="4317729" y="2443999"/>
+          <a:off x="4317729" y="2508339"/>
           <a:ext cx="892000" cy="446000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2864,7 +3111,7 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="4317729" y="2443999"/>
+        <a:off x="4317729" y="2508339"/>
         <a:ext cx="892000" cy="446000"/>
       </dsp:txXfrm>
     </dsp:sp>
@@ -5056,16 +5303,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>342900</xdr:colOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:rowOff>57150</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>66675</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5372,10 +5619,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G39"/>
+  <dimension ref="A1:H44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5388,7 +5635,7 @@
     <col min="7" max="7" width="38.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5405,7 +5652,7 @@
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -5413,7 +5660,7 @@
         <v>11</v>
       </c>
       <c r="C2" t="s">
-        <v>12</v>
+        <v>55</v>
       </c>
       <c r="D2" t="s">
         <v>13</v>
@@ -5422,7 +5669,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:8">
       <c r="B3" t="s">
         <v>14</v>
       </c>
@@ -5436,12 +5683,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:8">
       <c r="B4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C4" t="s">
         <v>46</v>
-      </c>
-      <c r="C4" t="s">
-        <v>47</v>
       </c>
       <c r="E4" t="s">
         <v>25</v>
@@ -5450,7 +5697,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:8">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -5458,7 +5705,7 @@
         <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>12</v>
+        <v>55</v>
       </c>
       <c r="D5" t="s">
         <v>13</v>
@@ -5467,7 +5714,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:8">
       <c r="B6" t="s">
         <v>14</v>
       </c>
@@ -5484,51 +5731,51 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:8">
       <c r="B7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E7" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:8">
       <c r="B8" t="s">
         <v>15</v>
       </c>
       <c r="C8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E8" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:8">
       <c r="B9" t="s">
         <v>16</v>
       </c>
       <c r="C9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E9" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:8">
       <c r="B10" t="s">
         <v>17</v>
       </c>
       <c r="C10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E10" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:8">
       <c r="A11" t="s">
         <v>3</v>
       </c>
@@ -5536,7 +5783,7 @@
         <v>11</v>
       </c>
       <c r="C11" t="s">
-        <v>12</v>
+        <v>55</v>
       </c>
       <c r="D11" t="s">
         <v>13</v>
@@ -5545,7 +5792,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:8">
       <c r="B12" t="s">
         <v>14</v>
       </c>
@@ -5562,20 +5809,20 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:8">
       <c r="B13" t="s">
+        <v>48</v>
+      </c>
+      <c r="C13" t="s">
         <v>49</v>
-      </c>
-      <c r="C13" t="s">
-        <v>50</v>
       </c>
       <c r="E13" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:8">
       <c r="A14" t="s">
-        <v>4</v>
+        <v>54</v>
       </c>
       <c r="B14" t="s">
         <v>11</v>
@@ -5589,54 +5836,63 @@
       <c r="E14" t="s">
         <v>25</v>
       </c>
+      <c r="H14" t="s">
+        <v>56</v>
+      </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:8">
       <c r="B15" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="C15" t="s">
-        <v>34</v>
-      </c>
-      <c r="E15" t="s">
-        <v>25</v>
-      </c>
-      <c r="F15" t="s">
-        <v>18</v>
+        <v>33</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:8">
       <c r="B16" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C16" t="s">
-        <v>12</v>
-      </c>
-      <c r="E16" t="s">
-        <v>25</v>
+        <v>57</v>
       </c>
     </row>
     <row r="17" spans="1:7">
+      <c r="A17" t="s">
+        <v>4</v>
+      </c>
       <c r="B17" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="C17" t="s">
         <v>12</v>
+      </c>
+      <c r="D17" t="s">
+        <v>13</v>
+      </c>
+      <c r="E17" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="18" spans="1:7">
       <c r="B18" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C18" t="s">
         <v>50</v>
+      </c>
+      <c r="E18" t="s">
+        <v>25</v>
+      </c>
+      <c r="F18" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="19" spans="1:7">
       <c r="B19" t="s">
-        <v>30</v>
+        <v>61</v>
       </c>
       <c r="C19" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="E19" t="s">
         <v>25</v>
@@ -5644,49 +5900,37 @@
     </row>
     <row r="20" spans="1:7">
       <c r="B20" t="s">
-        <v>31</v>
+        <v>51</v>
       </c>
       <c r="C20" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
     </row>
     <row r="21" spans="1:7">
-      <c r="A21" t="s">
-        <v>5</v>
-      </c>
       <c r="B21" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="C21" t="s">
-        <v>12</v>
-      </c>
-      <c r="D21" t="s">
-        <v>13</v>
-      </c>
-      <c r="E21" t="s">
-        <v>25</v>
+        <v>53</v>
       </c>
     </row>
     <row r="22" spans="1:7">
       <c r="B22" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="C22" t="s">
-        <v>39</v>
-      </c>
-      <c r="E22" t="s">
-        <v>25</v>
-      </c>
-      <c r="F22" t="s">
-        <v>18</v>
+        <v>58</v>
+      </c>
+      <c r="G22" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="23" spans="1:7">
       <c r="B23" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="C23" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="E23" t="s">
         <v>25</v>
@@ -5694,48 +5938,57 @@
     </row>
     <row r="24" spans="1:7">
       <c r="B24" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="C24" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
     </row>
     <row r="25" spans="1:7">
       <c r="B25" t="s">
-        <v>38</v>
+        <v>60</v>
       </c>
       <c r="C25" t="s">
-        <v>48</v>
+        <v>33</v>
       </c>
     </row>
     <row r="26" spans="1:7">
+      <c r="A26" t="s">
+        <v>5</v>
+      </c>
       <c r="B26" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="C26" t="s">
-        <v>48</v>
+        <v>12</v>
+      </c>
+      <c r="D26" t="s">
+        <v>13</v>
+      </c>
+      <c r="E26" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="27" spans="1:7">
       <c r="B27" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="C27" t="s">
-        <v>48</v>
+        <v>38</v>
+      </c>
+      <c r="E27" t="s">
+        <v>25</v>
+      </c>
+      <c r="F27" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="28" spans="1:7">
-      <c r="A28" t="s">
-        <v>6</v>
-      </c>
       <c r="B28" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
       <c r="C28" t="s">
-        <v>12</v>
-      </c>
-      <c r="D28" t="s">
-        <v>13</v>
+        <v>38</v>
       </c>
       <c r="E28" t="s">
         <v>25</v>
@@ -5743,98 +5996,89 @@
     </row>
     <row r="29" spans="1:7">
       <c r="B29" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="C29" t="s">
-        <v>34</v>
-      </c>
-      <c r="E29" t="s">
-        <v>25</v>
-      </c>
-      <c r="F29" t="s">
-        <v>18</v>
-      </c>
-      <c r="G29" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
     </row>
     <row r="30" spans="1:7">
       <c r="B30" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="C30" t="s">
-        <v>12</v>
+        <v>47</v>
       </c>
     </row>
     <row r="31" spans="1:7">
       <c r="B31" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C31" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="32" spans="1:7">
-      <c r="A32" t="s">
-        <v>7</v>
-      </c>
       <c r="B32" t="s">
-        <v>11</v>
+        <v>30</v>
       </c>
       <c r="C32" t="s">
-        <v>12</v>
-      </c>
-      <c r="D32" t="s">
-        <v>13</v>
-      </c>
-      <c r="E32" t="s">
-        <v>25</v>
+        <v>47</v>
       </c>
     </row>
     <row r="33" spans="1:7">
+      <c r="A33" t="s">
+        <v>6</v>
+      </c>
       <c r="B33" t="s">
-        <v>36</v>
+        <v>11</v>
       </c>
       <c r="C33" t="s">
-        <v>39</v>
+        <v>12</v>
+      </c>
+      <c r="D33" t="s">
+        <v>13</v>
       </c>
       <c r="E33" t="s">
         <v>25</v>
-      </c>
-      <c r="F33" t="s">
-        <v>18</v>
-      </c>
-      <c r="G33" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="34" spans="1:7">
       <c r="B34" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="C34" t="s">
-        <v>48</v>
+        <v>33</v>
+      </c>
+      <c r="E34" t="s">
+        <v>25</v>
+      </c>
+      <c r="F34" t="s">
+        <v>18</v>
+      </c>
+      <c r="G34" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="35" spans="1:7">
       <c r="B35" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="C35" t="s">
-        <v>42</v>
+        <v>12</v>
       </c>
     </row>
     <row r="36" spans="1:7">
       <c r="B36" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C36" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="37" spans="1:7">
       <c r="A37" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="B37" t="s">
         <v>11</v>
@@ -5851,26 +6095,84 @@
     </row>
     <row r="38" spans="1:7">
       <c r="B38" t="s">
-        <v>19</v>
+        <v>35</v>
       </c>
       <c r="C38" t="s">
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="E38" t="s">
         <v>25</v>
       </c>
       <c r="F38" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="G38" t="s">
-        <v>22</v>
+        <v>42</v>
       </c>
     </row>
     <row r="39" spans="1:7">
       <c r="B39" t="s">
+        <v>40</v>
+      </c>
+      <c r="C39" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7">
+      <c r="B40" t="s">
+        <v>41</v>
+      </c>
+      <c r="C40" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7">
+      <c r="B41" t="s">
+        <v>32</v>
+      </c>
+      <c r="C41" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7">
+      <c r="A42" t="s">
+        <v>23</v>
+      </c>
+      <c r="B42" t="s">
+        <v>11</v>
+      </c>
+      <c r="C42" t="s">
+        <v>12</v>
+      </c>
+      <c r="D42" t="s">
+        <v>13</v>
+      </c>
+      <c r="E42" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7">
+      <c r="B43" t="s">
+        <v>19</v>
+      </c>
+      <c r="C43" t="s">
+        <v>20</v>
+      </c>
+      <c r="E43" t="s">
+        <v>25</v>
+      </c>
+      <c r="F43" t="s">
+        <v>21</v>
+      </c>
+      <c r="G43" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7">
+      <c r="B44" t="s">
         <v>24</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C44" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Adding more tables to mySql
</commit_message>
<xml_diff>
--- a/assets/doku/DB tables.xlsx
+++ b/assets/doku/DB tables.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="64">
   <si>
     <t>Table</t>
   </si>
@@ -201,7 +201,13 @@
     <t>category</t>
   </si>
   <si>
-    <t>item_price_range</t>
+    <t xml:space="preserve">item_price_from </t>
+  </si>
+  <si>
+    <t>item_price_to</t>
+  </si>
+  <si>
+    <t>decimal</t>
   </si>
 </sst>
 </file>
@@ -1861,8 +1867,8 @@
     <dgm:cxn modelId="{58D39FB8-3B72-436D-B378-75D5CFD0C8F7}" srcId="{90625BEE-1CE8-4E94-BD93-26C691FBA331}" destId="{862D7E0D-F0D4-41D7-97A9-5B92A6FAF196}" srcOrd="3" destOrd="0" parTransId="{03BF1FA9-C075-4FA8-BD05-B802322534A6}" sibTransId="{C266CAE2-4D1C-4F15-A627-AE1D114514FC}"/>
     <dgm:cxn modelId="{9B39BB91-BCA2-4F88-A888-A93460ACAC0D}" srcId="{656B0FA4-A7DA-4D70-9B17-633C6CD7B506}" destId="{A6185CF1-A6C9-4057-B034-F738C98E78D8}" srcOrd="0" destOrd="0" parTransId="{4FB2B5CC-B5E8-4444-9946-1293B3748920}" sibTransId="{E6879C87-8E8C-49ED-9950-ECD513F23E89}"/>
     <dgm:cxn modelId="{B0173BF3-1663-4869-9510-FF3E6ECDB80B}" type="presOf" srcId="{90625BEE-1CE8-4E94-BD93-26C691FBA331}" destId="{96CAB6C0-43D1-4509-B5E4-801A2235C3C0}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
+    <dgm:cxn modelId="{DCBE64CE-AD06-4484-A607-7AE8805AA703}" type="presOf" srcId="{50773849-F511-4835-AD5C-FC578FA128E4}" destId="{D09303C9-BCC6-4DD2-8E33-C0F1AE38C831}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
     <dgm:cxn modelId="{1901550F-B5B2-4B92-9703-D60185DDB73A}" type="presOf" srcId="{4E1CD3DD-F8B4-4A0F-97E8-1A1E5C772D18}" destId="{ACC15529-EE74-465D-8E76-84913ECA718C}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
-    <dgm:cxn modelId="{DCBE64CE-AD06-4484-A607-7AE8805AA703}" type="presOf" srcId="{50773849-F511-4835-AD5C-FC578FA128E4}" destId="{D09303C9-BCC6-4DD2-8E33-C0F1AE38C831}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
     <dgm:cxn modelId="{325DAB41-614B-4868-B08A-5032FB3CA0F3}" srcId="{50773849-F511-4835-AD5C-FC578FA128E4}" destId="{B56F1F7B-9CAF-4E3C-8845-E5A0D88E4AC1}" srcOrd="0" destOrd="0" parTransId="{237A5FB3-0392-40DF-98C3-051D76C85975}" sibTransId="{D9AC3E19-03F8-4B24-9C05-1F58DDABFDD4}"/>
     <dgm:cxn modelId="{A02A8C92-53D2-400A-8E31-C1D36C74C310}" type="presOf" srcId="{A6185CF1-A6C9-4057-B034-F738C98E78D8}" destId="{488D30EC-5368-42BE-91A5-E867C0D7A783}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
     <dgm:cxn modelId="{71E0349D-088D-4E65-A8C6-D6879D89E856}" type="presOf" srcId="{03BF1FA9-C075-4FA8-BD05-B802322534A6}" destId="{F2B1825C-8BC8-4111-A2C0-A0FBB338DE48}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/orgChart1"/>
@@ -1968,7 +1974,7 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="2605087" y="2321019"/>
+          <a:off x="2605087" y="2511519"/>
           <a:ext cx="2158641" cy="187320"/>
         </a:xfrm>
         <a:custGeom>
@@ -2029,7 +2035,7 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="2605087" y="2321019"/>
+          <a:off x="2605087" y="2511519"/>
           <a:ext cx="1079320" cy="187320"/>
         </a:xfrm>
         <a:custGeom>
@@ -2090,7 +2096,7 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="2248287" y="2954339"/>
+          <a:off x="2248287" y="3144839"/>
           <a:ext cx="133800" cy="410320"/>
         </a:xfrm>
         <a:custGeom>
@@ -2148,7 +2154,7 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="2559367" y="2321019"/>
+          <a:off x="2559367" y="2511519"/>
           <a:ext cx="91440" cy="187320"/>
         </a:xfrm>
         <a:custGeom>
@@ -2203,7 +2209,7 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="1168966" y="3587660"/>
+          <a:off x="1168966" y="3778160"/>
           <a:ext cx="133800" cy="410320"/>
         </a:xfrm>
         <a:custGeom>
@@ -2261,7 +2267,7 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="1480046" y="2954339"/>
+          <a:off x="1480046" y="3144839"/>
           <a:ext cx="91440" cy="187320"/>
         </a:xfrm>
         <a:custGeom>
@@ -2316,7 +2322,7 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="1525766" y="2321019"/>
+          <a:off x="1525766" y="2511519"/>
           <a:ext cx="1079320" cy="187320"/>
         </a:xfrm>
         <a:custGeom>
@@ -2377,7 +2383,7 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="446445" y="2321019"/>
+          <a:off x="446445" y="2511519"/>
           <a:ext cx="2158641" cy="187320"/>
         </a:xfrm>
         <a:custGeom>
@@ -2438,7 +2444,7 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="2159087" y="1875018"/>
+          <a:off x="2159087" y="2065518"/>
           <a:ext cx="892000" cy="446000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2503,7 +2509,7 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="2159087" y="1875018"/>
+        <a:off x="2159087" y="2065518"/>
         <a:ext cx="892000" cy="446000"/>
       </dsp:txXfrm>
     </dsp:sp>
@@ -2514,7 +2520,7 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="445" y="2508339"/>
+          <a:off x="445" y="2698839"/>
           <a:ext cx="892000" cy="446000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2579,7 +2585,7 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="445" y="2508339"/>
+        <a:off x="445" y="2698839"/>
         <a:ext cx="892000" cy="446000"/>
       </dsp:txXfrm>
     </dsp:sp>
@@ -2590,7 +2596,7 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="1079766" y="2508339"/>
+          <a:off x="1079766" y="2698839"/>
           <a:ext cx="892000" cy="446000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2655,7 +2661,7 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="1079766" y="2508339"/>
+        <a:off x="1079766" y="2698839"/>
         <a:ext cx="892000" cy="446000"/>
       </dsp:txXfrm>
     </dsp:sp>
@@ -2666,7 +2672,7 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="1079766" y="3141660"/>
+          <a:off x="1079766" y="3332160"/>
           <a:ext cx="892000" cy="446000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2731,7 +2737,7 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="1079766" y="3141660"/>
+        <a:off x="1079766" y="3332160"/>
         <a:ext cx="892000" cy="446000"/>
       </dsp:txXfrm>
     </dsp:sp>
@@ -2742,7 +2748,7 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="1302766" y="3774980"/>
+          <a:off x="1302766" y="3965480"/>
           <a:ext cx="892000" cy="446000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2807,7 +2813,7 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="1302766" y="3774980"/>
+        <a:off x="1302766" y="3965480"/>
         <a:ext cx="892000" cy="446000"/>
       </dsp:txXfrm>
     </dsp:sp>
@@ -2818,7 +2824,7 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="2159087" y="2508339"/>
+          <a:off x="2159087" y="2698839"/>
           <a:ext cx="892000" cy="446000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2883,7 +2889,7 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="2159087" y="2508339"/>
+        <a:off x="2159087" y="2698839"/>
         <a:ext cx="892000" cy="446000"/>
       </dsp:txXfrm>
     </dsp:sp>
@@ -2894,7 +2900,7 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="2382087" y="3141660"/>
+          <a:off x="2382087" y="3332160"/>
           <a:ext cx="892000" cy="446000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2959,7 +2965,7 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="2382087" y="3141660"/>
+        <a:off x="2382087" y="3332160"/>
         <a:ext cx="892000" cy="446000"/>
       </dsp:txXfrm>
     </dsp:sp>
@@ -2970,7 +2976,7 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="3238408" y="2508339"/>
+          <a:off x="3238408" y="2698839"/>
           <a:ext cx="892000" cy="446000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -3035,7 +3041,7 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="3238408" y="2508339"/>
+        <a:off x="3238408" y="2698839"/>
         <a:ext cx="892000" cy="446000"/>
       </dsp:txXfrm>
     </dsp:sp>
@@ -3046,7 +3052,7 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="4317729" y="2508339"/>
+          <a:off x="4317729" y="2698839"/>
           <a:ext cx="892000" cy="446000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -3111,7 +3117,7 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="4317729" y="2508339"/>
+        <a:off x="4317729" y="2698839"/>
         <a:ext cx="892000" cy="446000"/>
       </dsp:txXfrm>
     </dsp:sp>
@@ -5311,7 +5317,7 @@
     <xdr:to>
       <xdr:col>17</xdr:col>
       <xdr:colOff>571500</xdr:colOff>
-      <xdr:row>33</xdr:row>
+      <xdr:row>34</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -5619,10 +5625,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H44"/>
+  <dimension ref="A1:H45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5892,127 +5898,124 @@
         <v>61</v>
       </c>
       <c r="C19" t="s">
-        <v>50</v>
-      </c>
-      <c r="E19" t="s">
-        <v>25</v>
+        <v>63</v>
       </c>
     </row>
     <row r="20" spans="1:7">
       <c r="B20" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
       <c r="C20" t="s">
-        <v>52</v>
+        <v>63</v>
       </c>
     </row>
     <row r="21" spans="1:7">
       <c r="B21" t="s">
-        <v>27</v>
+        <v>51</v>
       </c>
       <c r="C21" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="22" spans="1:7">
       <c r="B22" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C22" t="s">
-        <v>58</v>
-      </c>
-      <c r="G22" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
     </row>
     <row r="23" spans="1:7">
       <c r="B23" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C23" t="s">
-        <v>47</v>
-      </c>
-      <c r="E23" t="s">
-        <v>25</v>
+        <v>58</v>
+      </c>
+      <c r="G23" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="24" spans="1:7">
       <c r="B24" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C24" t="s">
         <v>47</v>
+      </c>
+      <c r="E24" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="25" spans="1:7">
       <c r="B25" t="s">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="C25" t="s">
-        <v>33</v>
+        <v>47</v>
       </c>
     </row>
     <row r="26" spans="1:7">
-      <c r="A26" t="s">
-        <v>5</v>
-      </c>
       <c r="B26" t="s">
-        <v>11</v>
+        <v>60</v>
       </c>
       <c r="C26" t="s">
-        <v>12</v>
-      </c>
-      <c r="D26" t="s">
-        <v>13</v>
-      </c>
-      <c r="E26" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
     </row>
     <row r="27" spans="1:7">
+      <c r="A27" t="s">
+        <v>5</v>
+      </c>
       <c r="B27" t="s">
-        <v>35</v>
+        <v>11</v>
       </c>
       <c r="C27" t="s">
-        <v>38</v>
+        <v>12</v>
+      </c>
+      <c r="D27" t="s">
+        <v>13</v>
       </c>
       <c r="E27" t="s">
         <v>25</v>
-      </c>
-      <c r="F27" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="28" spans="1:7">
       <c r="B28" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C28" t="s">
         <v>38</v>
       </c>
       <c r="E28" t="s">
         <v>25</v>
+      </c>
+      <c r="F28" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="29" spans="1:7">
       <c r="B29" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C29" t="s">
         <v>38</v>
+      </c>
+      <c r="E29" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="30" spans="1:7">
       <c r="B30" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C30" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
     </row>
     <row r="31" spans="1:7">
       <c r="B31" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="C31" t="s">
         <v>47</v>
@@ -6020,159 +6023,167 @@
     </row>
     <row r="32" spans="1:7">
       <c r="B32" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C32" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="33" spans="1:7">
-      <c r="A33" t="s">
-        <v>6</v>
-      </c>
       <c r="B33" t="s">
-        <v>11</v>
+        <v>30</v>
       </c>
       <c r="C33" t="s">
-        <v>12</v>
-      </c>
-      <c r="D33" t="s">
-        <v>13</v>
-      </c>
-      <c r="E33" t="s">
-        <v>25</v>
+        <v>47</v>
       </c>
     </row>
     <row r="34" spans="1:7">
+      <c r="A34" t="s">
+        <v>6</v>
+      </c>
       <c r="B34" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="C34" t="s">
-        <v>33</v>
+        <v>12</v>
+      </c>
+      <c r="D34" t="s">
+        <v>13</v>
       </c>
       <c r="E34" t="s">
         <v>25</v>
-      </c>
-      <c r="F34" t="s">
-        <v>18</v>
-      </c>
-      <c r="G34" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="35" spans="1:7">
       <c r="B35" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C35" t="s">
-        <v>12</v>
+        <v>33</v>
+      </c>
+      <c r="E35" t="s">
+        <v>25</v>
+      </c>
+      <c r="F35" t="s">
+        <v>18</v>
+      </c>
+      <c r="G35" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="36" spans="1:7">
       <c r="B36" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C36" t="s">
-        <v>47</v>
+        <v>12</v>
       </c>
     </row>
     <row r="37" spans="1:7">
-      <c r="A37" t="s">
-        <v>7</v>
-      </c>
       <c r="B37" t="s">
-        <v>11</v>
+        <v>32</v>
       </c>
       <c r="C37" t="s">
-        <v>12</v>
-      </c>
-      <c r="D37" t="s">
-        <v>13</v>
-      </c>
-      <c r="E37" t="s">
-        <v>25</v>
+        <v>47</v>
       </c>
     </row>
     <row r="38" spans="1:7">
+      <c r="A38" t="s">
+        <v>7</v>
+      </c>
       <c r="B38" t="s">
-        <v>35</v>
+        <v>11</v>
       </c>
       <c r="C38" t="s">
-        <v>38</v>
+        <v>12</v>
+      </c>
+      <c r="D38" t="s">
+        <v>13</v>
       </c>
       <c r="E38" t="s">
         <v>25</v>
-      </c>
-      <c r="F38" t="s">
-        <v>18</v>
-      </c>
-      <c r="G38" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="39" spans="1:7">
       <c r="B39" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="C39" t="s">
-        <v>47</v>
+        <v>38</v>
+      </c>
+      <c r="E39" t="s">
+        <v>25</v>
+      </c>
+      <c r="F39" t="s">
+        <v>18</v>
+      </c>
+      <c r="G39" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="40" spans="1:7">
       <c r="B40" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C40" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
     </row>
     <row r="41" spans="1:7">
       <c r="B41" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="C41" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
     </row>
     <row r="42" spans="1:7">
-      <c r="A42" t="s">
-        <v>23</v>
-      </c>
       <c r="B42" t="s">
-        <v>11</v>
+        <v>32</v>
       </c>
       <c r="C42" t="s">
-        <v>12</v>
-      </c>
-      <c r="D42" t="s">
-        <v>13</v>
-      </c>
-      <c r="E42" t="s">
-        <v>25</v>
+        <v>47</v>
       </c>
     </row>
     <row r="43" spans="1:7">
+      <c r="A43" t="s">
+        <v>23</v>
+      </c>
       <c r="B43" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="C43" t="s">
-        <v>20</v>
+        <v>12</v>
+      </c>
+      <c r="D43" t="s">
+        <v>13</v>
       </c>
       <c r="E43" t="s">
         <v>25</v>
-      </c>
-      <c r="F43" t="s">
-        <v>21</v>
-      </c>
-      <c r="G43" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="44" spans="1:7">
       <c r="B44" t="s">
+        <v>19</v>
+      </c>
+      <c r="C44" t="s">
+        <v>20</v>
+      </c>
+      <c r="E44" t="s">
+        <v>25</v>
+      </c>
+      <c r="F44" t="s">
+        <v>21</v>
+      </c>
+      <c r="G44" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7">
+      <c r="B45" t="s">
         <v>24</v>
       </c>
-      <c r="C44" t="s">
+      <c r="C45" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>